<commit_message>
feat: add warm up
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
   <si>
     <t>int</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>children</t>
+  </si>
+  <si>
+    <t>warmUp</t>
+  </si>
+  <si>
+    <t>warmUpFindRange</t>
+  </si>
+  <si>
+    <t>warmUpAttackDamage</t>
+  </si>
+  <si>
+    <t>warmUpAttackTime</t>
   </si>
   <si>
     <t>buff的id</t>
@@ -240,6 +252,18 @@
   </si>
   <si>
     <t>分裂出来的小怪</t>
+  </si>
+  <si>
+    <t>暖机</t>
+  </si>
+  <si>
+    <t>暖机后的攻击范围</t>
+  </si>
+  <si>
+    <t>暖机后的攻击力</t>
+  </si>
+  <si>
+    <t>暖机后的攻速</t>
   </si>
   <si>
     <t>Language</t>
@@ -1512,12 +1536,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP35"/>
+  <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomLeft" activeCell="AE33" sqref="AE33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9416666666667" defaultRowHeight="14.5"/>
@@ -1548,7 +1572,11 @@
     <col min="27" max="27" width="10.9583333333333" style="2"/>
     <col min="28" max="28" width="10.9583333333333" style="1"/>
     <col min="29" max="29" width="10.9583333333333" style="2"/>
-    <col min="30" max="1024" width="10.9583333333333" style="1"/>
+    <col min="30" max="30" width="10.9583333333333" style="1"/>
+    <col min="31" max="31" width="24.1666666666667" style="1" customWidth="1"/>
+    <col min="32" max="32" width="25.2" style="1" customWidth="1"/>
+    <col min="33" max="33" width="20" style="1" customWidth="1"/>
+    <col min="34" max="1024" width="10.9583333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1" spans="1:42">
@@ -1639,10 +1667,18 @@
       <c r="AC1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
+      <c r="AD1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
@@ -1741,10 +1777,18 @@
       <c r="AC2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
+      <c r="AD2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
@@ -1757,96 +1801,104 @@
     </row>
     <row r="3" ht="105.2" customHeight="1" spans="1:42">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
@@ -1859,10 +1911,10 @@
     </row>
     <row r="4" ht="16.5" spans="3:3">
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:33">
       <c r="A5" s="2">
         <v>1001</v>
       </c>
@@ -1878,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1946,8 +1998,20 @@
       <c r="AC5" s="1">
         <v>0</v>
       </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:33">
       <c r="A6" s="2">
         <v>1002</v>
       </c>
@@ -1963,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -2031,8 +2095,20 @@
       <c r="AC6" s="1">
         <v>0</v>
       </c>
+      <c r="AD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:33">
       <c r="A7" s="2">
         <v>1003</v>
       </c>
@@ -2114,8 +2190,20 @@
       <c r="AC7" s="1">
         <v>0</v>
       </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:33">
       <c r="A8" s="2">
         <v>1004</v>
       </c>
@@ -2131,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -2199,8 +2287,20 @@
       <c r="AC8" s="1">
         <v>0</v>
       </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:33">
       <c r="A9" s="2">
         <v>1005</v>
       </c>
@@ -2281,8 +2381,20 @@
       <c r="AC9" s="1">
         <v>0</v>
       </c>
+      <c r="AD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:33">
       <c r="A10" s="2">
         <v>1006</v>
       </c>
@@ -2291,7 +2403,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1">
         <v>-1</v>
@@ -2365,8 +2477,20 @@
       <c r="AC10" s="1">
         <v>0</v>
       </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:33">
       <c r="A11" s="2">
         <v>1007</v>
       </c>
@@ -2375,7 +2499,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E11" s="1">
         <v>-1</v>
@@ -2449,8 +2573,20 @@
       <c r="AC11" s="1">
         <v>0</v>
       </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:33">
       <c r="A12" s="2">
         <v>1008</v>
       </c>
@@ -2459,7 +2595,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1">
         <v>-1</v>
@@ -2533,8 +2669,20 @@
       <c r="AC12" s="1">
         <v>0</v>
       </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:33">
       <c r="A13" s="2">
         <v>1009</v>
       </c>
@@ -2543,7 +2691,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E13" s="1">
         <v>-1</v>
@@ -2617,8 +2765,20 @@
       <c r="AC13" s="1">
         <v>0</v>
       </c>
+      <c r="AD13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:33">
       <c r="A14" s="2">
         <v>1010</v>
       </c>
@@ -2627,7 +2787,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1">
         <v>-1</v>
@@ -2701,8 +2861,20 @@
       <c r="AC14" s="1">
         <v>0</v>
       </c>
+      <c r="AD14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:33">
       <c r="A15" s="2">
         <v>1011</v>
       </c>
@@ -2711,7 +2883,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E15" s="1">
         <v>-1</v>
@@ -2785,8 +2957,20 @@
       <c r="AC15" s="1">
         <v>0</v>
       </c>
+      <c r="AD15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:33">
       <c r="A16" s="2">
         <v>1012</v>
       </c>
@@ -2795,7 +2979,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E16" s="1">
         <v>-1</v>
@@ -2869,8 +3053,20 @@
       <c r="AC16" s="1">
         <v>0</v>
       </c>
+      <c r="AD16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:33">
       <c r="A17" s="2">
         <v>1013</v>
       </c>
@@ -2879,7 +3075,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E17" s="1">
         <v>-1</v>
@@ -2953,8 +3149,20 @@
       <c r="AC17" s="1">
         <v>0</v>
       </c>
+      <c r="AD17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:33">
       <c r="A18" s="2">
         <v>1014</v>
       </c>
@@ -2963,7 +3171,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1">
         <v>-1</v>
@@ -3037,8 +3245,20 @@
       <c r="AC18" s="1">
         <v>0</v>
       </c>
+      <c r="AD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:33">
       <c r="A19" s="2">
         <v>2001</v>
       </c>
@@ -3047,7 +3267,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1">
         <v>0.3</v>
@@ -3056,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -3124,8 +3344,20 @@
       <c r="AC19" s="1">
         <v>0</v>
       </c>
+      <c r="AD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:33">
       <c r="A20" s="2">
         <v>2002</v>
       </c>
@@ -3134,7 +3366,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1">
         <v>0.3</v>
@@ -3143,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -3211,8 +3443,20 @@
       <c r="AC20" s="1">
         <v>0</v>
       </c>
+      <c r="AD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:33">
       <c r="A21" s="2">
         <v>2003</v>
       </c>
@@ -3221,7 +3465,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1">
         <v>0.3</v>
@@ -3230,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -3298,8 +3542,20 @@
       <c r="AC21" s="1">
         <v>0</v>
       </c>
+      <c r="AD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" ht="15.5" spans="1:29">
+    <row r="22" ht="15.5" spans="1:33">
       <c r="A22" s="1">
         <v>3001</v>
       </c>
@@ -3307,10 +3563,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
@@ -3319,7 +3575,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -3387,8 +3643,20 @@
       <c r="AC22" s="1">
         <v>0</v>
       </c>
+      <c r="AD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" ht="15.5" spans="1:29">
+    <row r="23" ht="15.5" spans="1:33">
       <c r="A23" s="1">
         <v>3002</v>
       </c>
@@ -3396,10 +3664,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1">
         <v>20</v>
@@ -3408,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
@@ -3476,8 +3744,20 @@
       <c r="AC23" s="1">
         <v>0</v>
       </c>
+      <c r="AD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" ht="15.5" spans="1:29">
+    <row r="24" ht="15.5" spans="1:33">
       <c r="A24" s="1">
         <v>3003</v>
       </c>
@@ -3485,10 +3765,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E24" s="1">
         <v>20</v>
@@ -3497,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -3565,8 +3845,20 @@
       <c r="AC24" s="1">
         <v>0</v>
       </c>
+      <c r="AD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:33">
       <c r="A25" s="1">
         <v>4001</v>
       </c>
@@ -3574,7 +3866,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E25" s="1">
         <v>-1</v>
@@ -3648,8 +3940,20 @@
       <c r="AC25" s="1">
         <v>0</v>
       </c>
+      <c r="AD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:33">
       <c r="A26" s="1">
         <v>4002</v>
       </c>
@@ -3657,7 +3961,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E26" s="1">
         <v>-1</v>
@@ -3731,8 +4035,20 @@
       <c r="AC26" s="1">
         <v>0</v>
       </c>
+      <c r="AD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:33">
       <c r="A27" s="1">
         <v>4003</v>
       </c>
@@ -3740,7 +4056,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1">
         <v>-1</v>
@@ -3814,8 +4130,20 @@
       <c r="AC27" s="1">
         <v>0</v>
       </c>
+      <c r="AD27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:33">
       <c r="A28" s="1">
         <v>4004</v>
       </c>
@@ -3823,7 +4151,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -3897,8 +4225,20 @@
       <c r="AC28" s="1">
         <v>0</v>
       </c>
+      <c r="AD28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:33">
       <c r="A29" s="1">
         <v>4005</v>
       </c>
@@ -3906,7 +4246,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E29" s="1">
         <v>3</v>
@@ -3980,8 +4320,20 @@
       <c r="AC29" s="1">
         <v>0</v>
       </c>
+      <c r="AD29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:33">
       <c r="A30" s="1">
         <v>4006</v>
       </c>
@@ -3989,7 +4341,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -4063,8 +4415,20 @@
       <c r="AC30" s="1">
         <v>0</v>
       </c>
+      <c r="AD30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:33">
       <c r="A31" s="1">
         <v>4007</v>
       </c>
@@ -4072,7 +4436,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -4146,8 +4510,20 @@
       <c r="AC31" s="1">
         <v>0</v>
       </c>
+      <c r="AD31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:33">
       <c r="A32" s="1">
         <v>4008</v>
       </c>
@@ -4155,7 +4531,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E32" s="1">
         <v>-1</v>
@@ -4229,16 +4605,28 @@
       <c r="AC32" s="1">
         <v>0</v>
       </c>
+      <c r="AD32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:33">
       <c r="A33" s="1">
-        <v>5001</v>
+        <v>4009</v>
       </c>
       <c r="B33" s="1">
-        <v>5001</v>
+        <v>4009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="E33" s="1">
         <v>-1</v>
@@ -4247,7 +4635,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -4301,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="Z33" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA33" s="1">
         <v>0</v>
@@ -4312,16 +4700,28 @@
       <c r="AC33" s="1">
         <v>0</v>
       </c>
+      <c r="AD33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>50</v>
+      </c>
+      <c r="AG33" s="1">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:33">
       <c r="A34" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B34" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E34" s="1">
         <v>-1</v>
@@ -4384,10 +4784,10 @@
         <v>0</v>
       </c>
       <c r="Z34" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB34" s="1">
         <v>0</v>
@@ -4395,16 +4795,28 @@
       <c r="AC34" s="1">
         <v>0</v>
       </c>
+      <c r="AD34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:33">
       <c r="A35" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B35" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E35" s="1">
         <v>-1</v>
@@ -4470,13 +4882,120 @@
         <v>0</v>
       </c>
       <c r="AA35" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33">
+      <c r="A36" s="1">
+        <v>5003</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5003</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+      <c r="U36" s="1">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1">
         <v>5</v>
       </c>
-      <c r="AC35" s="2">
+      <c r="AC36" s="2">
         <v>1001</v>
+      </c>
+      <c r="AD36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add multi hit damage
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>int</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>warmUpAttackTime</t>
+  </si>
+  <si>
+    <t>multiHit</t>
   </si>
   <si>
     <t>buff的id</t>
@@ -254,103 +257,116 @@
     <t>分裂出来的小怪</t>
   </si>
   <si>
+    <t>暖机时间（s）</t>
+  </si>
+  <si>
+    <t>暖机后的提升攻击范围
+最终攻击范围=原范围+提升范围</t>
+  </si>
+  <si>
+    <t>暖机后的提升攻击力
+最终攻击力=原攻击力+提升攻击力</t>
+  </si>
+  <si>
+    <t>暖机后的提升攻速
+最终攻速=原攻速-提升攻速</t>
+  </si>
+  <si>
+    <t>多段伤害
+触发的次数</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>B0A6C67D4A3AE05B102976883590F4ED</t>
+  </si>
+  <si>
+    <t>FF3268BA438E7D17853D88A2A6C8FB89</t>
+  </si>
+  <si>
+    <t>永久固定值加攻击力</t>
+  </si>
+  <si>
+    <t>永久百分比加攻击力</t>
+  </si>
+  <si>
+    <t>减少固定值攻击间隔</t>
+  </si>
+  <si>
+    <t>永久百分比降低攻击间隔</t>
+  </si>
+  <si>
+    <t>怪物受到伤害百分比提升</t>
+  </si>
+  <si>
+    <t>怪物减速</t>
+  </si>
+  <si>
+    <t>怪物永久百分比减速</t>
+  </si>
+  <si>
+    <t>永久固定加攻击范围</t>
+  </si>
+  <si>
+    <t>增加攻击范围百分比</t>
+  </si>
+  <si>
+    <t>永久百分比加攻击力1</t>
+  </si>
+  <si>
+    <t>75E610CC445049E89172F4B7F387FAFB</t>
+  </si>
+  <si>
+    <t>永久百分比加攻击力2</t>
+  </si>
+  <si>
+    <t>5813EE7E45E077985D984295FD40D837</t>
+  </si>
+  <si>
+    <t>永久百分比加攻击力3</t>
+  </si>
+  <si>
+    <t>39CC680245A50F9AE8DBA09F16A0D43C</t>
+  </si>
+  <si>
+    <t>buffAirdrop_name1</t>
+  </si>
+  <si>
+    <t>空投Buff1</t>
+  </si>
+  <si>
+    <t>buffAirdrop_name2</t>
+  </si>
+  <si>
+    <t>空投Buff2</t>
+  </si>
+  <si>
+    <t>buffAirdrop_name3</t>
+  </si>
+  <si>
+    <t>空投Buff3</t>
+  </si>
+  <si>
+    <t>增伤</t>
+  </si>
+  <si>
+    <t>物穿</t>
+  </si>
+  <si>
+    <t>削护甲</t>
+  </si>
+  <si>
+    <t>怪物禁锢</t>
+  </si>
+  <si>
+    <t>对空增伤</t>
+  </si>
+  <si>
     <t>暖机</t>
   </si>
   <si>
-    <t>暖机后的攻击范围</t>
-  </si>
-  <si>
-    <t>暖机后的攻击力</t>
-  </si>
-  <si>
-    <t>暖机后的攻速</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>B0A6C67D4A3AE05B102976883590F4ED</t>
-  </si>
-  <si>
-    <t>FF3268BA438E7D17853D88A2A6C8FB89</t>
-  </si>
-  <si>
-    <t>永久固定值加攻击力</t>
-  </si>
-  <si>
-    <t>永久百分比加攻击力</t>
-  </si>
-  <si>
-    <t>减少固定值攻击间隔</t>
-  </si>
-  <si>
-    <t>永久百分比降低攻击间隔</t>
-  </si>
-  <si>
-    <t>怪物受到伤害百分比提升</t>
-  </si>
-  <si>
-    <t>怪物减速</t>
-  </si>
-  <si>
-    <t>怪物永久百分比减速</t>
-  </si>
-  <si>
-    <t>永久固定加攻击范围</t>
-  </si>
-  <si>
-    <t>增加攻击范围百分比</t>
-  </si>
-  <si>
-    <t>永久百分比加攻击力1</t>
-  </si>
-  <si>
-    <t>75E610CC445049E89172F4B7F387FAFB</t>
-  </si>
-  <si>
-    <t>永久百分比加攻击力2</t>
-  </si>
-  <si>
-    <t>5813EE7E45E077985D984295FD40D837</t>
-  </si>
-  <si>
-    <t>永久百分比加攻击力3</t>
-  </si>
-  <si>
-    <t>39CC680245A50F9AE8DBA09F16A0D43C</t>
-  </si>
-  <si>
-    <t>buffAirdrop_name1</t>
-  </si>
-  <si>
-    <t>空投Buff1</t>
-  </si>
-  <si>
-    <t>buffAirdrop_name2</t>
-  </si>
-  <si>
-    <t>空投Buff2</t>
-  </si>
-  <si>
-    <t>buffAirdrop_name3</t>
-  </si>
-  <si>
-    <t>空投Buff3</t>
-  </si>
-  <si>
-    <t>增伤</t>
-  </si>
-  <si>
-    <t>物穿</t>
-  </si>
-  <si>
-    <t>削护甲</t>
-  </si>
-  <si>
-    <t>怪物禁锢</t>
-  </si>
-  <si>
-    <t>对空增伤</t>
+    <t>多段伤害</t>
   </si>
   <si>
     <t>复原力</t>
@@ -1536,12 +1552,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP36"/>
+  <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AE33" sqref="AE33"/>
+      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9416666666667" defaultRowHeight="14.5"/>
@@ -1679,7 +1695,9 @@
       <c r="AG1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="3"/>
+      <c r="AH1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
@@ -1789,7 +1807,9 @@
       <c r="AG2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="3"/>
+      <c r="AH2" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
@@ -1801,105 +1821,107 @@
     </row>
     <row r="3" ht="105.2" customHeight="1" spans="1:42">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AE3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AF3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AH3" s="3"/>
+      <c r="AG3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
@@ -1911,10 +1933,10 @@
     </row>
     <row r="4" ht="16.5" spans="3:3">
       <c r="C4" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:34">
       <c r="A5" s="2">
         <v>1001</v>
       </c>
@@ -1930,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -2010,8 +2032,11 @@
       <c r="AG5" s="1">
         <v>0</v>
       </c>
+      <c r="AH5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:34">
       <c r="A6" s="2">
         <v>1002</v>
       </c>
@@ -2027,7 +2052,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -2107,8 +2132,11 @@
       <c r="AG6" s="1">
         <v>0</v>
       </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:34">
       <c r="A7" s="2">
         <v>1003</v>
       </c>
@@ -2202,8 +2230,11 @@
       <c r="AG7" s="1">
         <v>0</v>
       </c>
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:34">
       <c r="A8" s="2">
         <v>1004</v>
       </c>
@@ -2219,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -2299,8 +2330,11 @@
       <c r="AG8" s="1">
         <v>0</v>
       </c>
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:34">
       <c r="A9" s="2">
         <v>1005</v>
       </c>
@@ -2393,8 +2427,11 @@
       <c r="AG9" s="1">
         <v>0</v>
       </c>
+      <c r="AH9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:34">
       <c r="A10" s="2">
         <v>1006</v>
       </c>
@@ -2403,7 +2440,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1">
         <v>-1</v>
@@ -2489,8 +2526,11 @@
       <c r="AG10" s="1">
         <v>0</v>
       </c>
+      <c r="AH10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:34">
       <c r="A11" s="2">
         <v>1007</v>
       </c>
@@ -2499,7 +2539,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1">
         <v>-1</v>
@@ -2585,8 +2625,11 @@
       <c r="AG11" s="1">
         <v>0</v>
       </c>
+      <c r="AH11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:34">
       <c r="A12" s="2">
         <v>1008</v>
       </c>
@@ -2595,7 +2638,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E12" s="1">
         <v>-1</v>
@@ -2681,8 +2724,11 @@
       <c r="AG12" s="1">
         <v>0</v>
       </c>
+      <c r="AH12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:34">
       <c r="A13" s="2">
         <v>1009</v>
       </c>
@@ -2691,7 +2737,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E13" s="1">
         <v>-1</v>
@@ -2777,8 +2823,11 @@
       <c r="AG13" s="1">
         <v>0</v>
       </c>
+      <c r="AH13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:34">
       <c r="A14" s="2">
         <v>1010</v>
       </c>
@@ -2787,7 +2836,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E14" s="1">
         <v>-1</v>
@@ -2873,8 +2922,11 @@
       <c r="AG14" s="1">
         <v>0</v>
       </c>
+      <c r="AH14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:34">
       <c r="A15" s="2">
         <v>1011</v>
       </c>
@@ -2883,7 +2935,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E15" s="1">
         <v>-1</v>
@@ -2969,8 +3021,11 @@
       <c r="AG15" s="1">
         <v>0</v>
       </c>
+      <c r="AH15" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:34">
       <c r="A16" s="2">
         <v>1012</v>
       </c>
@@ -2979,7 +3034,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E16" s="1">
         <v>-1</v>
@@ -3065,8 +3120,11 @@
       <c r="AG16" s="1">
         <v>0</v>
       </c>
+      <c r="AH16" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:34">
       <c r="A17" s="2">
         <v>1013</v>
       </c>
@@ -3075,7 +3133,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E17" s="1">
         <v>-1</v>
@@ -3161,8 +3219,11 @@
       <c r="AG17" s="1">
         <v>0</v>
       </c>
+      <c r="AH17" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:34">
       <c r="A18" s="2">
         <v>1014</v>
       </c>
@@ -3171,7 +3232,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1">
         <v>-1</v>
@@ -3257,8 +3318,11 @@
       <c r="AG18" s="1">
         <v>0</v>
       </c>
+      <c r="AH18" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:34">
       <c r="A19" s="2">
         <v>2001</v>
       </c>
@@ -3267,7 +3331,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E19" s="1">
         <v>0.3</v>
@@ -3276,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -3356,8 +3420,11 @@
       <c r="AG19" s="1">
         <v>0</v>
       </c>
+      <c r="AH19" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:34">
       <c r="A20" s="2">
         <v>2002</v>
       </c>
@@ -3366,7 +3433,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1">
         <v>0.3</v>
@@ -3375,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -3455,8 +3522,11 @@
       <c r="AG20" s="1">
         <v>0</v>
       </c>
+      <c r="AH20" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:34">
       <c r="A21" s="2">
         <v>2003</v>
       </c>
@@ -3465,7 +3535,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1">
         <v>0.3</v>
@@ -3474,7 +3544,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -3554,8 +3624,11 @@
       <c r="AG21" s="1">
         <v>0</v>
       </c>
+      <c r="AH21" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" ht="15.5" spans="1:33">
+    <row r="22" ht="15.5" spans="1:34">
       <c r="A22" s="1">
         <v>3001</v>
       </c>
@@ -3563,10 +3636,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
@@ -3575,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -3655,8 +3728,11 @@
       <c r="AG22" s="1">
         <v>0</v>
       </c>
+      <c r="AH22" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" ht="15.5" spans="1:33">
+    <row r="23" ht="15.5" spans="1:34">
       <c r="A23" s="1">
         <v>3002</v>
       </c>
@@ -3664,10 +3740,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1">
         <v>20</v>
@@ -3676,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
@@ -3756,8 +3832,11 @@
       <c r="AG23" s="1">
         <v>0</v>
       </c>
+      <c r="AH23" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" ht="15.5" spans="1:33">
+    <row r="24" ht="15.5" spans="1:34">
       <c r="A24" s="1">
         <v>3003</v>
       </c>
@@ -3765,10 +3844,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1">
         <v>20</v>
@@ -3777,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -3857,8 +3936,11 @@
       <c r="AG24" s="1">
         <v>0</v>
       </c>
+      <c r="AH24" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:34">
       <c r="A25" s="1">
         <v>4001</v>
       </c>
@@ -3866,7 +3948,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1">
         <v>-1</v>
@@ -3952,8 +4034,11 @@
       <c r="AG25" s="1">
         <v>0</v>
       </c>
+      <c r="AH25" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:34">
       <c r="A26" s="1">
         <v>4002</v>
       </c>
@@ -3961,7 +4046,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E26" s="1">
         <v>-1</v>
@@ -4047,8 +4132,11 @@
       <c r="AG26" s="1">
         <v>0</v>
       </c>
+      <c r="AH26" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:34">
       <c r="A27" s="1">
         <v>4003</v>
       </c>
@@ -4056,7 +4144,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E27" s="1">
         <v>-1</v>
@@ -4142,8 +4230,11 @@
       <c r="AG27" s="1">
         <v>0</v>
       </c>
+      <c r="AH27" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:34">
       <c r="A28" s="1">
         <v>4004</v>
       </c>
@@ -4151,7 +4242,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -4237,8 +4328,11 @@
       <c r="AG28" s="1">
         <v>0</v>
       </c>
+      <c r="AH28" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:34">
       <c r="A29" s="1">
         <v>4005</v>
       </c>
@@ -4246,7 +4340,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E29" s="1">
         <v>3</v>
@@ -4332,8 +4426,11 @@
       <c r="AG29" s="1">
         <v>0</v>
       </c>
+      <c r="AH29" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:34">
       <c r="A30" s="1">
         <v>4006</v>
       </c>
@@ -4341,7 +4438,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -4427,8 +4524,11 @@
       <c r="AG30" s="1">
         <v>0</v>
       </c>
+      <c r="AH30" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:34">
       <c r="A31" s="1">
         <v>4007</v>
       </c>
@@ -4436,7 +4536,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -4522,8 +4622,11 @@
       <c r="AG31" s="1">
         <v>0</v>
       </c>
+      <c r="AH31" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:34">
       <c r="A32" s="1">
         <v>4008</v>
       </c>
@@ -4531,7 +4634,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1">
         <v>-1</v>
@@ -4617,8 +4720,11 @@
       <c r="AG32" s="1">
         <v>0</v>
       </c>
+      <c r="AH32" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:34">
       <c r="A33" s="1">
         <v>4009</v>
       </c>
@@ -4626,7 +4732,7 @@
         <v>4009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="E33" s="1">
         <v>-1</v>
@@ -4712,16 +4818,19 @@
       <c r="AG33" s="1">
         <v>0.2</v>
       </c>
+      <c r="AH33" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:34">
       <c r="A34" s="1">
-        <v>5001</v>
+        <v>4010</v>
       </c>
       <c r="B34" s="1">
-        <v>5001</v>
+        <v>4010</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E34" s="1">
         <v>-1</v>
@@ -4730,93 +4839,96 @@
         <v>1</v>
       </c>
       <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0</v>
+      </c>
+      <c r="X34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="1">
         <v>2</v>
       </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-      <c r="J34" s="1">
-        <v>0</v>
-      </c>
-      <c r="K34" s="1">
-        <v>0</v>
-      </c>
-      <c r="L34" s="1">
-        <v>0</v>
-      </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1">
-        <v>0</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="1">
-        <v>0</v>
-      </c>
-      <c r="R34" s="1">
-        <v>0</v>
-      </c>
-      <c r="S34" s="1">
-        <v>0</v>
-      </c>
-      <c r="T34" s="1">
-        <v>0</v>
-      </c>
-      <c r="U34" s="1">
-        <v>0</v>
-      </c>
-      <c r="V34" s="1">
-        <v>0</v>
-      </c>
-      <c r="W34" s="1">
-        <v>0</v>
-      </c>
-      <c r="X34" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="1">
-        <v>25</v>
-      </c>
-      <c r="AA34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG34" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:34">
       <c r="A35" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B35" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E35" s="1">
         <v>-1</v>
@@ -4879,10 +4991,10 @@
         <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA35" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="1">
         <v>0</v>
@@ -4902,16 +5014,19 @@
       <c r="AG35" s="1">
         <v>0</v>
       </c>
+      <c r="AH35" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:34">
       <c r="A36" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B36" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E36" s="1">
         <v>-1</v>
@@ -4977,24 +5092,125 @@
         <v>0</v>
       </c>
       <c r="AA36" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34">
+      <c r="A37" s="1">
+        <v>5003</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5003</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0</v>
+      </c>
+      <c r="U37" s="1">
+        <v>0</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0</v>
+      </c>
+      <c r="W37" s="1">
+        <v>0</v>
+      </c>
+      <c r="X37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1">
         <v>5</v>
       </c>
-      <c r="AC36" s="2">
+      <c r="AC37" s="2">
         <v>1001</v>
       </c>
-      <c r="AD36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG36" s="2">
+      <c r="AD37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: flying first buff
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
   <si>
     <t>int</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>multiHit</t>
+  </si>
+  <si>
+    <t>flyFirst</t>
   </si>
   <si>
     <t>buff的id</t>
@@ -276,6 +279,11 @@
 触发的次数</t>
   </si>
   <si>
+    <t>优先对空
+0 没有
+1 有</t>
+  </si>
+  <si>
     <t>Language</t>
   </si>
   <si>
@@ -367,6 +375,9 @@
   </si>
   <si>
     <t>多段伤害</t>
+  </si>
+  <si>
+    <t>优先对空</t>
   </si>
   <si>
     <t>复原力</t>
@@ -1552,12 +1563,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP37"/>
+  <dimension ref="A1:AP38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomLeft" activeCell="AG49" sqref="AG49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9416666666667" defaultRowHeight="14.5"/>
@@ -1698,7 +1709,9 @@
       <c r="AH1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AI1" s="3"/>
+      <c r="AI1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
@@ -1810,7 +1823,9 @@
       <c r="AH2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AI2" s="3"/>
+      <c r="AI2" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
@@ -1821,108 +1836,110 @@
     </row>
     <row r="3" ht="105.2" customHeight="1" spans="1:42">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI3" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
@@ -1933,10 +1950,10 @@
     </row>
     <row r="4" ht="16.5" spans="3:3">
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="2">
         <v>1001</v>
       </c>
@@ -1952,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -2035,8 +2052,11 @@
       <c r="AH5" s="1">
         <v>0</v>
       </c>
+      <c r="AI5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="2">
         <v>1002</v>
       </c>
@@ -2052,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -2135,8 +2155,11 @@
       <c r="AH6" s="1">
         <v>0</v>
       </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="2">
         <v>1003</v>
       </c>
@@ -2233,8 +2256,11 @@
       <c r="AH7" s="1">
         <v>0</v>
       </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="2">
         <v>1004</v>
       </c>
@@ -2250,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -2333,8 +2359,11 @@
       <c r="AH8" s="1">
         <v>0</v>
       </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="2">
         <v>1005</v>
       </c>
@@ -2430,8 +2459,11 @@
       <c r="AH9" s="1">
         <v>0</v>
       </c>
+      <c r="AI9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="2">
         <v>1006</v>
       </c>
@@ -2440,7 +2472,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1">
         <v>-1</v>
@@ -2529,8 +2561,11 @@
       <c r="AH10" s="1">
         <v>0</v>
       </c>
+      <c r="AI10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="2">
         <v>1007</v>
       </c>
@@ -2539,7 +2574,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E11" s="1">
         <v>-1</v>
@@ -2628,8 +2663,11 @@
       <c r="AH11" s="1">
         <v>0</v>
       </c>
+      <c r="AI11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="2">
         <v>1008</v>
       </c>
@@ -2638,7 +2676,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E12" s="1">
         <v>-1</v>
@@ -2727,8 +2765,11 @@
       <c r="AH12" s="1">
         <v>0</v>
       </c>
+      <c r="AI12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:35">
       <c r="A13" s="2">
         <v>1009</v>
       </c>
@@ -2737,7 +2778,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E13" s="1">
         <v>-1</v>
@@ -2826,8 +2867,11 @@
       <c r="AH13" s="1">
         <v>0</v>
       </c>
+      <c r="AI13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:35">
       <c r="A14" s="2">
         <v>1010</v>
       </c>
@@ -2836,7 +2880,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E14" s="1">
         <v>-1</v>
@@ -2925,8 +2969,11 @@
       <c r="AH14" s="1">
         <v>0</v>
       </c>
+      <c r="AI14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:35">
       <c r="A15" s="2">
         <v>1011</v>
       </c>
@@ -2935,7 +2982,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1">
         <v>-1</v>
@@ -3024,8 +3071,11 @@
       <c r="AH15" s="1">
         <v>0</v>
       </c>
+      <c r="AI15" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:35">
       <c r="A16" s="2">
         <v>1012</v>
       </c>
@@ -3034,7 +3084,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1">
         <v>-1</v>
@@ -3123,8 +3173,11 @@
       <c r="AH16" s="1">
         <v>0</v>
       </c>
+      <c r="AI16" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:35">
       <c r="A17" s="2">
         <v>1013</v>
       </c>
@@ -3133,7 +3186,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E17" s="1">
         <v>-1</v>
@@ -3222,8 +3275,11 @@
       <c r="AH17" s="1">
         <v>0</v>
       </c>
+      <c r="AI17" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:35">
       <c r="A18" s="2">
         <v>1014</v>
       </c>
@@ -3232,7 +3288,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1">
         <v>-1</v>
@@ -3321,8 +3377,11 @@
       <c r="AH18" s="1">
         <v>0</v>
       </c>
+      <c r="AI18" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:35">
       <c r="A19" s="2">
         <v>2001</v>
       </c>
@@ -3331,7 +3390,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1">
         <v>0.3</v>
@@ -3340,7 +3399,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -3423,8 +3482,11 @@
       <c r="AH19" s="1">
         <v>0</v>
       </c>
+      <c r="AI19" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:34">
+    <row r="20" spans="1:35">
       <c r="A20" s="2">
         <v>2002</v>
       </c>
@@ -3433,7 +3495,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1">
         <v>0.3</v>
@@ -3442,7 +3504,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -3525,8 +3587,11 @@
       <c r="AH20" s="1">
         <v>0</v>
       </c>
+      <c r="AI20" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:34">
+    <row r="21" spans="1:35">
       <c r="A21" s="2">
         <v>2003</v>
       </c>
@@ -3535,7 +3600,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1">
         <v>0.3</v>
@@ -3544,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -3627,8 +3692,11 @@
       <c r="AH21" s="1">
         <v>0</v>
       </c>
+      <c r="AI21" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" ht="15.5" spans="1:34">
+    <row r="22" ht="15.5" spans="1:35">
       <c r="A22" s="1">
         <v>3001</v>
       </c>
@@ -3636,10 +3704,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
@@ -3648,7 +3716,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -3731,8 +3799,11 @@
       <c r="AH22" s="1">
         <v>0</v>
       </c>
+      <c r="AI22" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" ht="15.5" spans="1:34">
+    <row r="23" ht="15.5" spans="1:35">
       <c r="A23" s="1">
         <v>3002</v>
       </c>
@@ -3740,10 +3811,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E23" s="1">
         <v>20</v>
@@ -3752,7 +3823,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
@@ -3835,8 +3906,11 @@
       <c r="AH23" s="1">
         <v>0</v>
       </c>
+      <c r="AI23" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" ht="15.5" spans="1:34">
+    <row r="24" ht="15.5" spans="1:35">
       <c r="A24" s="1">
         <v>3003</v>
       </c>
@@ -3844,10 +3918,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E24" s="1">
         <v>20</v>
@@ -3856,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -3939,8 +4013,11 @@
       <c r="AH24" s="1">
         <v>0</v>
       </c>
+      <c r="AI24" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>4001</v>
       </c>
@@ -3948,7 +4025,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E25" s="1">
         <v>-1</v>
@@ -4037,8 +4114,11 @@
       <c r="AH25" s="1">
         <v>0</v>
       </c>
+      <c r="AI25" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>4002</v>
       </c>
@@ -4046,7 +4126,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1">
         <v>-1</v>
@@ -4135,8 +4215,11 @@
       <c r="AH26" s="1">
         <v>0</v>
       </c>
+      <c r="AI26" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:34">
+    <row r="27" spans="1:35">
       <c r="A27" s="1">
         <v>4003</v>
       </c>
@@ -4144,7 +4227,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1">
         <v>-1</v>
@@ -4233,8 +4316,11 @@
       <c r="AH27" s="1">
         <v>0</v>
       </c>
+      <c r="AI27" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:34">
+    <row r="28" spans="1:35">
       <c r="A28" s="1">
         <v>4004</v>
       </c>
@@ -4242,7 +4328,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -4331,8 +4417,11 @@
       <c r="AH28" s="1">
         <v>0</v>
       </c>
+      <c r="AI28" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:34">
+    <row r="29" spans="1:35">
       <c r="A29" s="1">
         <v>4005</v>
       </c>
@@ -4340,7 +4429,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E29" s="1">
         <v>3</v>
@@ -4429,8 +4518,11 @@
       <c r="AH29" s="1">
         <v>0</v>
       </c>
+      <c r="AI29" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:34">
+    <row r="30" spans="1:35">
       <c r="A30" s="1">
         <v>4006</v>
       </c>
@@ -4438,7 +4530,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -4527,8 +4619,11 @@
       <c r="AH30" s="1">
         <v>0</v>
       </c>
+      <c r="AI30" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:35">
       <c r="A31" s="1">
         <v>4007</v>
       </c>
@@ -4536,7 +4631,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -4625,8 +4720,11 @@
       <c r="AH31" s="1">
         <v>0</v>
       </c>
+      <c r="AI31" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:34">
+    <row r="32" spans="1:35">
       <c r="A32" s="1">
         <v>4008</v>
       </c>
@@ -4634,7 +4732,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E32" s="1">
         <v>-1</v>
@@ -4723,8 +4821,11 @@
       <c r="AH32" s="1">
         <v>0</v>
       </c>
+      <c r="AI32" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:34">
+    <row r="33" spans="1:35">
       <c r="A33" s="1">
         <v>4009</v>
       </c>
@@ -4732,7 +4833,7 @@
         <v>4009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E33" s="1">
         <v>-1</v>
@@ -4821,8 +4922,11 @@
       <c r="AH33" s="1">
         <v>0</v>
       </c>
+      <c r="AI33" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:34">
+    <row r="34" spans="1:35">
       <c r="A34" s="1">
         <v>4010</v>
       </c>
@@ -4830,7 +4934,7 @@
         <v>4010</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1">
         <v>-1</v>
@@ -4919,16 +5023,19 @@
       <c r="AH34" s="1">
         <v>2</v>
       </c>
+      <c r="AI34" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:34">
+    <row r="35" spans="1:35">
       <c r="A35" s="1">
-        <v>5001</v>
+        <v>4011</v>
       </c>
       <c r="B35" s="1">
-        <v>5001</v>
+        <v>4011</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1">
         <v>-1</v>
@@ -4937,7 +5044,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -4991,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA35" s="1">
         <v>0</v>
@@ -5017,16 +5124,19 @@
       <c r="AH35" s="1">
         <v>0</v>
       </c>
+      <c r="AI35" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:34">
+    <row r="36" spans="1:35">
       <c r="A36" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B36" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E36" s="1">
         <v>-1</v>
@@ -5089,10 +5199,10 @@
         <v>0</v>
       </c>
       <c r="Z36" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA36" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB36" s="1">
         <v>0</v>
@@ -5115,16 +5225,19 @@
       <c r="AH36" s="1">
         <v>0</v>
       </c>
+      <c r="AI36" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:34">
+    <row r="37" spans="1:35">
       <c r="A37" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B37" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1">
         <v>-1</v>
@@ -5190,27 +5303,131 @@
         <v>0</v>
       </c>
       <c r="AA37" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35">
+      <c r="A38" s="1">
+        <v>5003</v>
+      </c>
+      <c r="B38" s="1">
+        <v>5003</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>0</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
+      <c r="U38" s="1">
+        <v>0</v>
+      </c>
+      <c r="V38" s="1">
+        <v>0</v>
+      </c>
+      <c r="W38" s="1">
+        <v>0</v>
+      </c>
+      <c r="X38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="1">
         <v>5</v>
       </c>
-      <c r="AC37" s="2">
+      <c r="AC38" s="2">
         <v>1001</v>
       </c>
-      <c r="AD37" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG37" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="1">
+      <c r="AD38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update dark dragon tower
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="118">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -382,6 +382,15 @@
   </si>
   <si>
     <t xml:space="preserve">暗龙娘1法穿3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">暗龙娘4物穿1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">暗龙娘4物穿2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">暗龙娘4物穿3</t>
   </si>
 </sst>
 </file>
@@ -591,7 +600,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,12 +791,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK41"/>
+  <dimension ref="A1:AMK44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="V42" activeCellId="0" sqref="V42:V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7941,6 +7950,309 @@
         <v>0</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>4015</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>4015</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="W42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>4016</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>4016</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" s="10" t="n">
+        <v>40</v>
+      </c>
+      <c r="W43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>4017</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>4017</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="W44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ44" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat：update water dragon 1—2
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="119">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t xml:space="preserve">暗龙娘4物穿3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水龙娘2法穿3</t>
   </si>
 </sst>
 </file>
@@ -791,12 +794,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK44"/>
+  <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="V42" activeCellId="0" sqref="V42:V44"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="X47" activeCellId="0" sqref="X47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8253,6 +8256,107 @@
         <v>0</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>4018</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>4014</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X45" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat:update tower and dragon icon
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t xml:space="preserve">水龙娘2法穿3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火龙娘眩晕</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火龙娘减速1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火龙娘减速2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火龙娘减速3</t>
   </si>
 </sst>
 </file>
@@ -794,12 +806,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK45"/>
+  <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="X47" activeCellId="0" sqref="X47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8261,7 +8273,7 @@
         <v>4018</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>4014</v>
+        <v>4018</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>118</v>
@@ -8354,6 +8366,413 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>4019</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>4019</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" s="1" t="n">
+        <v>-999</v>
+      </c>
+      <c r="S46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>4020</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>4020</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" s="10" t="n">
+        <v>-50</v>
+      </c>
+      <c r="S47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>4021</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>4021</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" s="10" t="n">
+        <v>-75</v>
+      </c>
+      <c r="S48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>4022</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>4022</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" s="10" t="n">
+        <v>-100</v>
+      </c>
+      <c r="S49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update soil dragon tower1——3
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -808,10 +808,10 @@
   </sheetPr>
   <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="R51" activeCellId="0" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8515,7 +8515,7 @@
         <v>0</v>
       </c>
       <c r="R47" s="10" t="n">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="S47" s="1" t="n">
         <v>0</v>
@@ -8617,7 +8617,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="10" t="n">
-        <v>-75</v>
+        <v>-20</v>
       </c>
       <c r="S48" s="1" t="n">
         <v>0</v>
@@ -8719,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="R49" s="10" t="n">
-        <v>-100</v>
+        <v>-30</v>
       </c>
       <c r="S49" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
feat：update buff excel change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="125">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">attackDamage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attackFixDamage</t>
   </si>
   <si>
     <t xml:space="preserve">attackDamagePercent</t>
@@ -179,6 +182,9 @@
   <si>
     <t xml:space="preserve">
     伤害数值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">固定伤害数值提升</t>
   </si>
   <si>
     <t xml:space="preserve">    伤害数值 百分比</t>
@@ -806,12 +812,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK49"/>
+  <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="R51" activeCellId="0" sqref="R51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -824,29 +830,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="7.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="35" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="6.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="24.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="20"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1026" min="36" style="1" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -931,10 +937,10 @@
       <c r="AA1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD1" s="3" t="s">
@@ -944,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG1" s="3" t="s">
         <v>2</v>
@@ -953,18 +959,21 @@
         <v>2</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AK1" s="3"/>
+      <c r="AK1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="AL1" s="3"/>
       <c r="AM1" s="3"/>
       <c r="AN1" s="3"/>
       <c r="AO1" s="3"/>
       <c r="AP1" s="3"/>
       <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -1024,13 +1033,13 @@
       <c r="S2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="W2" s="3" t="s">
@@ -1075,134 +1084,140 @@
       <c r="AJ2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="3"/>
+      <c r="AK2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
       <c r="AN2" s="3"/>
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="L3" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="S3" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="S3" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="T3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AC3" s="5" t="s">
+      <c r="AB3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AC3" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="AD3" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="AE3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF3" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="AF3" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="AG3" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AJ3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK3" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
       <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="n">
@@ -1230,15 +1245,12 @@
       <c r="J5" s="1" t="n">
         <v>-2</v>
       </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M5" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" s="1" t="n">
         <v>0</v>
       </c>
@@ -1306,6 +1318,9 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1325,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="n">
@@ -1334,15 +1349,12 @@
       <c r="J6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M6" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="N6" s="1" t="n">
         <v>0</v>
       </c>
@@ -1410,6 +1422,9 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1436,9 +1451,6 @@
       <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L7" s="1" t="n">
         <v>0</v>
       </c>
@@ -1446,11 +1458,11 @@
         <v>0</v>
       </c>
       <c r="N7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="O7" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
@@ -1512,6 +1524,9 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1531,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>2</v>
@@ -1539,9 +1554,6 @@
       <c r="J8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L8" s="1" t="n">
         <v>0</v>
       </c>
@@ -1564,11 +1576,11 @@
         <v>0</v>
       </c>
       <c r="S8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1" t="n">
         <v>-0.5</v>
       </c>
-      <c r="T8" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="U8" s="1" t="n">
         <v>0</v>
       </c>
@@ -1615,6 +1627,9 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1639,9 +1654,6 @@
       <c r="J9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L9" s="1" t="n">
         <v>0</v>
       </c>
@@ -1715,6 +1727,9 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1727,7 +1742,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>-1</v>
@@ -1741,9 +1756,7 @@
       <c r="J10" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="K10" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="K10" s="10"/>
       <c r="L10" s="1" t="n">
         <v>0</v>
       </c>
@@ -1817,6 +1830,9 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1829,7 +1845,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>-1</v>
@@ -1843,12 +1859,9 @@
       <c r="J11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="10" t="n">
+      <c r="L11" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="L11" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
       </c>
@@ -1919,6 +1932,9 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1931,7 +1947,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>-1</v>
@@ -1945,9 +1961,6 @@
       <c r="J12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L12" s="1" t="n">
         <v>0</v>
       </c>
@@ -1957,12 +1970,12 @@
       <c r="N12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O12" s="10" t="n">
+      <c r="O12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10" t="n">
         <v>-0.01</v>
       </c>
-      <c r="P12" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Q12" s="1" t="n">
         <v>0</v>
       </c>
@@ -2021,6 +2034,9 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2033,7 +2049,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>-1</v>
@@ -2047,9 +2063,6 @@
       <c r="J13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K13" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L13" s="1" t="n">
         <v>0</v>
       </c>
@@ -2062,12 +2075,12 @@
       <c r="O13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P13" s="10" t="n">
+      <c r="P13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10" t="n">
         <v>-20</v>
       </c>
-      <c r="Q13" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="R13" s="1" t="n">
         <v>0</v>
       </c>
@@ -2123,6 +2136,9 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2135,7 +2151,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>-1</v>
@@ -2149,9 +2165,6 @@
       <c r="J14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L14" s="1" t="n">
         <v>0</v>
       </c>
@@ -2179,12 +2192,12 @@
       <c r="T14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="U14" s="10" t="n">
+      <c r="U14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="V14" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W14" s="1" t="n">
         <v>0</v>
       </c>
@@ -2225,6 +2238,9 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2237,7 +2253,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>-1</v>
@@ -2251,9 +2267,6 @@
       <c r="J15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K15" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L15" s="1" t="n">
         <v>0</v>
       </c>
@@ -2272,12 +2285,12 @@
       <c r="Q15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R15" s="10" t="n">
+      <c r="R15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="S15" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T15" s="1" t="n">
         <v>0</v>
       </c>
@@ -2327,6 +2340,9 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2339,7 +2355,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>-1</v>
@@ -2353,9 +2369,6 @@
       <c r="J16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K16" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" s="1" t="n">
         <v>0</v>
       </c>
@@ -2377,12 +2390,12 @@
       <c r="R16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S16" s="10" t="n">
+      <c r="S16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="10" t="n">
         <v>-60</v>
       </c>
-      <c r="T16" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="U16" s="1" t="n">
         <v>0</v>
       </c>
@@ -2429,6 +2442,9 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2441,7 +2457,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>-1</v>
@@ -2455,15 +2471,12 @@
       <c r="J17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="10" t="n">
+      <c r="L17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="M17" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="N17" s="1" t="n">
         <v>0</v>
       </c>
@@ -2531,6 +2544,9 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2543,7 +2559,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>-1</v>
@@ -2557,18 +2573,15 @@
       <c r="J18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K18" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M18" s="10" t="n">
+      <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="N18" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="O18" s="1" t="n">
         <v>0</v>
       </c>
@@ -2633,6 +2646,9 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2645,29 +2661,27 @@
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E19" s="12" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I19" s="12" t="n">
         <v>1</v>
       </c>
       <c r="J19" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="K19" s="12" t="n">
-        <v>0</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K19" s="12"/>
       <c r="L19" s="12" t="n">
         <v>0</v>
       </c>
@@ -2743,7 +2757,9 @@
       <c r="AJ19" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AK19" s="12"/>
+      <c r="AK19" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="AL19" s="12"/>
       <c r="AM19" s="12"/>
       <c r="AN19" s="12"/>
@@ -3732,39 +3748,38 @@
       <c r="AMI19" s="12"/>
       <c r="AMJ19" s="12"/>
       <c r="AMK19" s="12"/>
+      <c r="AML19" s="12"/>
     </row>
     <row r="20" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="n">
         <v>2002</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E20" s="12" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="I20" s="12" t="n">
         <v>1</v>
       </c>
       <c r="J20" s="12" t="n">
-        <v>15</v>
-      </c>
-      <c r="K20" s="12" t="n">
-        <v>0</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="K20" s="12"/>
       <c r="L20" s="12" t="n">
         <v>0</v>
       </c>
@@ -3840,7 +3855,9 @@
       <c r="AJ20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AK20" s="12"/>
+      <c r="AK20" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="AL20" s="12"/>
       <c r="AM20" s="12"/>
       <c r="AN20" s="12"/>
@@ -4829,39 +4846,38 @@
       <c r="AMI20" s="12"/>
       <c r="AMJ20" s="12"/>
       <c r="AMK20" s="12"/>
+      <c r="AML20" s="12"/>
     </row>
     <row r="21" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="n">
         <v>2003</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>2001</v>
+        <v>2003</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E21" s="12" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>1</v>
       </c>
       <c r="J21" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="K21" s="12" t="n">
-        <v>0</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="K21" s="12"/>
       <c r="L21" s="12" t="n">
         <v>0</v>
       </c>
@@ -4937,7 +4953,9 @@
       <c r="AJ21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AK21" s="12"/>
+      <c r="AK21" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="AL21" s="12"/>
       <c r="AM21" s="12"/>
       <c r="AN21" s="12"/>
@@ -5926,6 +5944,7 @@
       <c r="AMI21" s="12"/>
       <c r="AMJ21" s="12"/>
       <c r="AMK21" s="12"/>
+      <c r="AML21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -5935,10 +5954,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>20</v>
@@ -5947,7 +5966,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>1</v>
@@ -5955,12 +5974,9 @@
       <c r="J22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K22" s="10" t="n">
+      <c r="L22" s="10" t="n">
         <v>2000</v>
       </c>
-      <c r="L22" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
       </c>
@@ -6031,6 +6047,9 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6042,10 +6061,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>20</v>
@@ -6054,7 +6073,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>1</v>
@@ -6062,18 +6081,15 @@
       <c r="J23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K23" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1" t="n">
+      <c r="L23" s="10" t="n">
         <v>0</v>
       </c>
       <c r="M23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="N23" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="O23" s="1" t="n">
         <v>0</v>
       </c>
@@ -6138,6 +6154,9 @@
         <v>0</v>
       </c>
       <c r="AJ23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6149,10 +6168,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>20</v>
@@ -6161,7 +6180,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>1</v>
@@ -6169,10 +6188,7 @@
       <c r="J24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K24" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1" t="n">
+      <c r="L24" s="10" t="n">
         <v>0</v>
       </c>
       <c r="M24" s="1" t="n">
@@ -6185,11 +6201,11 @@
         <v>0</v>
       </c>
       <c r="P24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1" t="n">
         <v>-2000</v>
       </c>
-      <c r="Q24" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="R24" s="1" t="n">
         <v>0</v>
       </c>
@@ -6245,6 +6261,9 @@
         <v>0</v>
       </c>
       <c r="AJ24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6256,7 +6275,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>-1</v>
@@ -6270,9 +6289,6 @@
       <c r="J25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K25" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L25" s="1" t="n">
         <v>0</v>
       </c>
@@ -6301,11 +6317,11 @@
         <v>0</v>
       </c>
       <c r="U25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="V25" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W25" s="1" t="n">
         <v>0</v>
       </c>
@@ -6346,6 +6362,9 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6357,7 +6376,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>-1</v>
@@ -6371,9 +6390,6 @@
       <c r="J26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L26" s="1" t="n">
         <v>0</v>
       </c>
@@ -6411,11 +6427,11 @@
         <v>0</v>
       </c>
       <c r="X26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="Y26" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Z26" s="1" t="n">
         <v>0</v>
       </c>
@@ -6447,6 +6463,9 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6458,7 +6477,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>-1</v>
@@ -6472,9 +6491,6 @@
       <c r="J27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K27" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L27" s="1" t="n">
         <v>0</v>
       </c>
@@ -6506,11 +6522,11 @@
         <v>0</v>
       </c>
       <c r="V27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="W27" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="X27" s="1" t="n">
         <v>0</v>
       </c>
@@ -6548,6 +6564,9 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6559,7 +6578,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>3</v>
@@ -6573,9 +6592,6 @@
       <c r="J28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K28" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L28" s="1" t="n">
         <v>0</v>
       </c>
@@ -6616,11 +6632,11 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Z28" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AA28" s="1" t="n">
         <v>0</v>
       </c>
@@ -6649,6 +6665,9 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6660,7 +6679,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>3</v>
@@ -6674,9 +6693,6 @@
       <c r="J29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L29" s="1" t="n">
         <v>0</v>
       </c>
@@ -6711,11 +6727,11 @@
         <v>0</v>
       </c>
       <c r="W29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="X29" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Y29" s="1" t="n">
         <v>0</v>
       </c>
@@ -6750,6 +6766,9 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6761,7 +6780,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>3</v>
@@ -6775,9 +6794,6 @@
       <c r="J30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K30" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L30" s="1" t="n">
         <v>0</v>
       </c>
@@ -6797,11 +6813,11 @@
         <v>0</v>
       </c>
       <c r="R30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1" t="n">
         <v>-30</v>
       </c>
-      <c r="S30" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T30" s="1" t="n">
         <v>0</v>
       </c>
@@ -6851,6 +6867,9 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6862,7 +6881,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>1</v>
@@ -6876,9 +6895,6 @@
       <c r="J31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K31" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L31" s="1" t="n">
         <v>0</v>
       </c>
@@ -6898,11 +6914,11 @@
         <v>0</v>
       </c>
       <c r="R31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" s="1" t="n">
         <v>-999</v>
       </c>
-      <c r="S31" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T31" s="1" t="n">
         <v>0</v>
       </c>
@@ -6952,6 +6968,9 @@
         <v>0</v>
       </c>
       <c r="AJ31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6963,7 +6982,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>-1</v>
@@ -6977,9 +6996,6 @@
       <c r="J32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K32" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L32" s="1" t="n">
         <v>0</v>
       </c>
@@ -7023,11 +7039,11 @@
         <v>0</v>
       </c>
       <c r="Z32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="AA32" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AB32" s="1" t="n">
         <v>0</v>
       </c>
@@ -7053,6 +7069,9 @@
         <v>0</v>
       </c>
       <c r="AJ32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7064,7 +7083,7 @@
         <v>4009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>-1</v>
@@ -7078,9 +7097,6 @@
       <c r="J33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K33" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L33" s="1" t="n">
         <v>0</v>
       </c>
@@ -7139,21 +7155,24 @@
         <v>0</v>
       </c>
       <c r="AE33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AF33" s="1" t="n">
+      <c r="AG33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AG33" s="1" t="n">
+      <c r="AH33" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="AH33" s="1" t="n">
+      <c r="AI33" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="AI33" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AJ33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7165,7 +7184,7 @@
         <v>4010</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>-1</v>
@@ -7179,9 +7198,6 @@
       <c r="J34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K34" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L34" s="1" t="n">
         <v>0</v>
       </c>
@@ -7252,9 +7268,12 @@
         <v>0</v>
       </c>
       <c r="AI34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AJ34" s="1" t="n">
+      <c r="AK34" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7266,7 +7285,7 @@
         <v>4011</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E35" s="1" t="n">
         <v>-1</v>
@@ -7280,9 +7299,6 @@
       <c r="J35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K35" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L35" s="1" t="n">
         <v>0</v>
       </c>
@@ -7356,6 +7372,9 @@
         <v>0</v>
       </c>
       <c r="AJ35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7367,7 +7386,7 @@
         <v>5001</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>-1</v>
@@ -7381,9 +7400,6 @@
       <c r="J36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K36" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L36" s="1" t="n">
         <v>0</v>
       </c>
@@ -7430,11 +7446,11 @@
         <v>0</v>
       </c>
       <c r="AA36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="AB36" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AC36" s="1" t="n">
         <v>0</v>
       </c>
@@ -7457,6 +7473,9 @@
         <v>0</v>
       </c>
       <c r="AJ36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7468,7 +7487,7 @@
         <v>5002</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>-1</v>
@@ -7482,9 +7501,6 @@
       <c r="J37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L37" s="1" t="n">
         <v>0</v>
       </c>
@@ -7534,11 +7550,11 @@
         <v>0</v>
       </c>
       <c r="AB37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AC37" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AD37" s="1" t="n">
         <v>0</v>
       </c>
@@ -7558,6 +7574,9 @@
         <v>0</v>
       </c>
       <c r="AJ37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK37" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7569,7 +7588,7 @@
         <v>5003</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>-1</v>
@@ -7583,9 +7602,6 @@
       <c r="J38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K38" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L38" s="1" t="n">
         <v>0</v>
       </c>
@@ -7638,14 +7654,14 @@
         <v>0</v>
       </c>
       <c r="AC38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AD38" s="2" t="n">
+      <c r="AE38" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="AE38" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="AF38" s="2" t="n">
         <v>0</v>
       </c>
@@ -7655,10 +7671,13 @@
       <c r="AH38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI38" s="1" t="n">
+      <c r="AI38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AJ38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7670,7 +7689,7 @@
         <v>4012</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>-1</v>
@@ -7684,9 +7703,6 @@
       <c r="J39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K39" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L39" s="1" t="n">
         <v>0</v>
       </c>
@@ -7723,12 +7739,12 @@
       <c r="W39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X39" s="10" t="n">
+      <c r="X39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="Y39" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Z39" s="1" t="n">
         <v>0</v>
       </c>
@@ -7760,6 +7776,9 @@
         <v>0</v>
       </c>
       <c r="AJ39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7771,7 +7790,7 @@
         <v>4013</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>-1</v>
@@ -7785,9 +7804,6 @@
       <c r="J40" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K40" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L40" s="1" t="n">
         <v>0</v>
       </c>
@@ -7824,12 +7840,12 @@
       <c r="W40" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X40" s="10" t="n">
+      <c r="X40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="Y40" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Z40" s="1" t="n">
         <v>0</v>
       </c>
@@ -7861,6 +7877,9 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7872,7 +7891,7 @@
         <v>4014</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>-1</v>
@@ -7886,9 +7905,6 @@
       <c r="J41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K41" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L41" s="1" t="n">
         <v>0</v>
       </c>
@@ -7925,12 +7941,12 @@
       <c r="W41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X41" s="10" t="n">
+      <c r="X41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="Y41" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Z41" s="1" t="n">
         <v>0</v>
       </c>
@@ -7962,6 +7978,9 @@
         <v>0</v>
       </c>
       <c r="AJ41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7973,7 +7992,7 @@
         <v>4015</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>-1</v>
@@ -7987,9 +8006,6 @@
       <c r="J42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K42" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L42" s="1" t="n">
         <v>0</v>
       </c>
@@ -8020,12 +8036,12 @@
       <c r="U42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="V42" s="10" t="n">
+      <c r="V42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="W42" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="X42" s="1" t="n">
         <v>0</v>
       </c>
@@ -8063,6 +8079,9 @@
         <v>0</v>
       </c>
       <c r="AJ42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8074,7 +8093,7 @@
         <v>4016</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>-1</v>
@@ -8088,9 +8107,6 @@
       <c r="J43" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K43" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L43" s="1" t="n">
         <v>0</v>
       </c>
@@ -8121,12 +8137,12 @@
       <c r="U43" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="V43" s="10" t="n">
+      <c r="V43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="W43" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="X43" s="1" t="n">
         <v>0</v>
       </c>
@@ -8164,6 +8180,9 @@
         <v>0</v>
       </c>
       <c r="AJ43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8175,7 +8194,7 @@
         <v>4017</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>-1</v>
@@ -8189,9 +8208,6 @@
       <c r="J44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K44" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L44" s="1" t="n">
         <v>0</v>
       </c>
@@ -8222,12 +8238,12 @@
       <c r="U44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="V44" s="10" t="n">
+      <c r="V44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="W44" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="X44" s="1" t="n">
         <v>0</v>
       </c>
@@ -8265,6 +8281,9 @@
         <v>0</v>
       </c>
       <c r="AJ44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK44" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8276,7 +8295,7 @@
         <v>4018</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>-1</v>
@@ -8290,9 +8309,6 @@
       <c r="J45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K45" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L45" s="1" t="n">
         <v>0</v>
       </c>
@@ -8329,12 +8345,12 @@
       <c r="W45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X45" s="10" t="n">
+      <c r="X45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="Y45" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Z45" s="1" t="n">
         <v>0</v>
       </c>
@@ -8366,6 +8382,9 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8377,7 +8396,7 @@
         <v>4019</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>1</v>
@@ -8391,9 +8410,6 @@
       <c r="J46" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K46" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L46" s="1" t="n">
         <v>0</v>
       </c>
@@ -8413,11 +8429,11 @@
         <v>0</v>
       </c>
       <c r="R46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1" t="n">
         <v>-999</v>
       </c>
-      <c r="S46" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T46" s="1" t="n">
         <v>0</v>
       </c>
@@ -8467,6 +8483,9 @@
         <v>0</v>
       </c>
       <c r="AJ46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8479,7 +8498,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>1</v>
@@ -8493,9 +8512,6 @@
       <c r="J47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K47" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L47" s="1" t="n">
         <v>0</v>
       </c>
@@ -8514,12 +8530,12 @@
       <c r="Q47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R47" s="10" t="n">
+      <c r="R47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" s="10" t="n">
         <v>-10</v>
       </c>
-      <c r="S47" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T47" s="1" t="n">
         <v>0</v>
       </c>
@@ -8569,6 +8585,9 @@
         <v>0</v>
       </c>
       <c r="AJ47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8581,7 +8600,7 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E48" s="1" t="n">
         <v>1</v>
@@ -8595,9 +8614,6 @@
       <c r="J48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K48" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L48" s="1" t="n">
         <v>0</v>
       </c>
@@ -8616,12 +8632,12 @@
       <c r="Q48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R48" s="10" t="n">
+      <c r="R48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="10" t="n">
         <v>-20</v>
       </c>
-      <c r="S48" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T48" s="1" t="n">
         <v>0</v>
       </c>
@@ -8671,6 +8687,9 @@
         <v>0</v>
       </c>
       <c r="AJ48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8683,7 +8702,7 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>1</v>
@@ -8697,9 +8716,6 @@
       <c r="J49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K49" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="L49" s="1" t="n">
         <v>0</v>
       </c>
@@ -8718,12 +8734,12 @@
       <c r="Q49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R49" s="10" t="n">
+      <c r="R49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" s="10" t="n">
         <v>-30</v>
       </c>
-      <c r="S49" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="T49" s="1" t="n">
         <v>0</v>
       </c>
@@ -8773,6 +8789,9 @@
         <v>0</v>
       </c>
       <c r="AJ49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：fix buff location and logo_anim
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t xml:space="preserve">光龙娘7 加攻击1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100|100|0</t>
   </si>
   <si>
     <t xml:space="preserve">光龙娘7 加攻击2</t>
@@ -885,10 +888,10 @@
   </sheetPr>
   <dimension ref="A1:AML64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="AB38" activeCellId="0" sqref="AB38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K53" activeCellId="0" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8887,7 +8890,7 @@
         <v>91</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I50" s="17" t="n">
         <v>1</v>
@@ -9975,7 +9978,7 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E51" s="1" t="n">
         <v>3</v>
@@ -9987,7 +9990,7 @@
         <v>94</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I51" s="1" t="n">
         <v>1</v>
@@ -11075,7 +11078,7 @@
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>3</v>
@@ -11087,7 +11090,7 @@
         <v>96</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I52" s="1" t="n">
         <v>1</v>
@@ -12175,7 +12178,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>-1</v>
@@ -12187,7 +12190,7 @@
         <v>91</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I53" s="1" t="n">
         <v>1</v>
@@ -13273,7 +13276,7 @@
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>-1</v>
@@ -13285,7 +13288,7 @@
         <v>94</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I54" s="1" t="n">
         <v>1</v>
@@ -14371,7 +14374,7 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E55" s="1" t="n">
         <v>-1</v>
@@ -14383,7 +14386,7 @@
         <v>96</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I55" s="1" t="n">
         <v>1</v>
@@ -15469,7 +15472,7 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E56" s="1" t="n">
         <v>6</v>
@@ -15481,7 +15484,7 @@
         <v>91</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I56" s="1" t="n">
         <v>1</v>
@@ -16567,7 +16570,7 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>6</v>
@@ -16579,7 +16582,7 @@
         <v>94</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I57" s="1" t="n">
         <v>1</v>
@@ -17665,7 +17668,7 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>6</v>
@@ -17677,7 +17680,7 @@
         <v>96</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I58" s="1" t="n">
         <v>1</v>
@@ -18763,7 +18766,7 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>-1</v>
@@ -18775,7 +18778,7 @@
         <v>91</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I59" s="1" t="n">
         <v>1</v>
@@ -19863,7 +19866,7 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E60" s="1" t="n">
         <v>-1</v>
@@ -19875,7 +19878,7 @@
         <v>94</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I60" s="1" t="n">
         <v>1</v>
@@ -20963,7 +20966,7 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E61" s="1" t="n">
         <v>-1</v>
@@ -20975,7 +20978,7 @@
         <v>96</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I61" s="1" t="n">
         <v>1</v>
@@ -22063,7 +22066,7 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E62" s="1" t="n">
         <v>-1</v>
@@ -22075,7 +22078,7 @@
         <v>91</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I62" s="1" t="n">
         <v>1</v>
@@ -23161,7 +23164,7 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>-1</v>
@@ -23173,7 +23176,7 @@
         <v>94</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I63" s="1" t="n">
         <v>1</v>
@@ -24259,7 +24262,7 @@
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>-1</v>
@@ -24271,7 +24274,7 @@
         <v>96</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I64" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
feat: update buff language UI
调整暖机buff，更新多语言，调整UI
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B033E690-7F39-491A-A8F0-AA98005D8049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24753" windowHeight="10480" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -517,14 +521,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -534,11 +532,13 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -546,23 +546,27 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -570,161 +574,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DejaVu Sans"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="DejaVu Sans"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="DejaVu Sans"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="DejaVu Sans"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="DejaVu Sans"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DejaVu Sans"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,7 +593,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
@@ -751,7 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,194 +615,8 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -982,251 +650,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1286,57 +712,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1410,6 +789,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1467,7 +849,7 @@
         <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1518,56 +900,55 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.65"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.10833333333333" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.7166666666667" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="3" customWidth="1"/>
     <col min="3" max="4" width="19" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.3833333333333" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="3" customWidth="1"/>
     <col min="7" max="8" width="32" style="3" customWidth="1"/>
     <col min="9" max="9" width="10" style="3" customWidth="1"/>
     <col min="10" max="10" width="13" style="3" customWidth="1"/>
-    <col min="11" max="12" width="19.1083333333333" style="3" customWidth="1"/>
-    <col min="13" max="13" width="9.88333333333333" style="3" customWidth="1"/>
-    <col min="14" max="15" width="11.3833333333333" style="3" customWidth="1"/>
+    <col min="11" max="12" width="19.125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.875" style="3" customWidth="1"/>
+    <col min="14" max="15" width="11.375" style="3" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="3" customWidth="1"/>
     <col min="17" max="17" width="16.5" style="3" customWidth="1"/>
-    <col min="18" max="18" width="11.2166666666667" style="3" customWidth="1"/>
-    <col min="19" max="19" width="6.21666666666667" style="3" customWidth="1"/>
-    <col min="20" max="20" width="12.3833333333333" style="3" customWidth="1"/>
-    <col min="21" max="21" width="7.83333333333333" style="3" customWidth="1"/>
-    <col min="22" max="22" width="11.2166666666667" style="3" customWidth="1"/>
+    <col min="18" max="18" width="11.25" style="3" customWidth="1"/>
+    <col min="19" max="19" width="6.25" style="3" customWidth="1"/>
+    <col min="20" max="20" width="12.375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="7.875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="11.25" style="3" customWidth="1"/>
     <col min="23" max="23" width="11" style="3"/>
-    <col min="24" max="24" width="13.8333333333333" style="3" customWidth="1"/>
+    <col min="24" max="24" width="13.875" style="3" customWidth="1"/>
     <col min="25" max="26" width="11" style="3"/>
-    <col min="27" max="27" width="24.2166666666667" style="3" customWidth="1"/>
+    <col min="27" max="27" width="24.25" style="3" customWidth="1"/>
     <col min="28" max="28" width="11" style="3"/>
     <col min="29" max="29" width="11" style="4"/>
     <col min="30" max="30" width="11" style="3"/>
     <col min="31" max="31" width="11" style="4"/>
     <col min="32" max="32" width="11" style="3"/>
-    <col min="33" max="33" width="24.1083333333333" style="3" customWidth="1"/>
-    <col min="34" max="34" width="25.2166666666667" style="3" customWidth="1"/>
+    <col min="33" max="33" width="24.125" style="3" customWidth="1"/>
+    <col min="34" max="34" width="25.25" style="3" customWidth="1"/>
     <col min="35" max="35" width="20" style="3" customWidth="1"/>
     <col min="36" max="1026" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1" spans="1:44">
+    <row r="1" spans="1:44" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1068,7 @@
       <c r="AQ1" s="5"/>
       <c r="AR1" s="5"/>
     </row>
-    <row r="2" ht="24.75" customHeight="1" spans="1:44">
+    <row r="2" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1807,7 +1188,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" ht="105" customHeight="1" spans="1:44">
+    <row r="3" spans="1:44" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1927,12 +1308,12 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" ht="15.3" spans="3:3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>1001</v>
       </c>
@@ -2036,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>1002</v>
       </c>
@@ -2140,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>1003</v>
       </c>
@@ -2242,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1004</v>
       </c>
@@ -2345,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>1005</v>
       </c>
@@ -2445,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>1006</v>
       </c>
@@ -2548,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>1007</v>
       </c>
@@ -2650,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>1008</v>
       </c>
@@ -2752,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>1009</v>
       </c>
@@ -2854,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>1010</v>
       </c>
@@ -2956,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>1011</v>
       </c>
@@ -3058,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>1012</v>
       </c>
@@ -3160,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>1013</v>
       </c>
@@ -3262,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>1014</v>
       </c>
@@ -3364,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" spans="1:1026">
+    <row r="19" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>2001</v>
       </c>
@@ -4462,7 +3843,7 @@
       <c r="AMK19" s="11"/>
       <c r="AML19" s="11"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:1026">
+    <row r="20" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>2002</v>
       </c>
@@ -5560,7 +4941,7 @@
       <c r="AMK20" s="11"/>
       <c r="AML20" s="11"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:1026">
+    <row r="21" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>2003</v>
       </c>
@@ -6658,7 +6039,7 @@
       <c r="AMK21" s="11"/>
       <c r="AML21" s="11"/>
     </row>
-    <row r="22" ht="15" spans="1:37">
+    <row r="22" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>3001</v>
       </c>
@@ -6765,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" ht="15" spans="1:37">
+    <row r="23" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>3002</v>
       </c>
@@ -6872,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" ht="15" spans="1:37">
+    <row r="24" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>3003</v>
       </c>
@@ -6979,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>4001</v>
       </c>
@@ -7080,7 +6461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>4002</v>
       </c>
@@ -7181,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>4003</v>
       </c>
@@ -7282,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>4004</v>
       </c>
@@ -7383,7 +6764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>4005</v>
       </c>
@@ -7484,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>4006</v>
       </c>
@@ -7585,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>4007</v>
       </c>
@@ -7686,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>4008</v>
       </c>
@@ -7787,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>4009</v>
       </c>
@@ -7870,7 +7251,7 @@
         <v>0</v>
       </c>
       <c r="AF33" s="3">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="AG33" s="3">
         <v>1</v>
@@ -7888,7 +7269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>4010</v>
       </c>
@@ -7989,7 +7370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>4011</v>
       </c>
@@ -8090,7 +7471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>5001</v>
       </c>
@@ -8191,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>5002</v>
       </c>
@@ -8292,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>5003</v>
       </c>
@@ -8393,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>4012</v>
       </c>
@@ -8494,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>4013</v>
       </c>
@@ -8595,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>4014</v>
       </c>
@@ -8696,7 +8077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>4015</v>
       </c>
@@ -8797,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>4016</v>
       </c>
@@ -8898,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>4017</v>
       </c>
@@ -8999,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>4018</v>
       </c>
@@ -9100,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>4019</v>
       </c>
@@ -9201,7 +8582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>4020</v>
       </c>
@@ -9303,7 +8684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>4021</v>
       </c>
@@ -9405,7 +8786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>4022</v>
       </c>
@@ -9507,7 +8888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" s="2" customFormat="1" spans="1:1026">
+    <row r="50" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14">
         <v>4023</v>
       </c>
@@ -10607,7 +9988,7 @@
       <c r="AMK50" s="15"/>
       <c r="AML50" s="15"/>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>4024</v>
       </c>
@@ -10718,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>4025</v>
       </c>
@@ -10829,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>4026</v>
       </c>
@@ -10937,7 +10318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>4027</v>
       </c>
@@ -11045,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>4028</v>
       </c>
@@ -11153,7 +10534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>4029</v>
       </c>
@@ -11260,7 +10641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>4030</v>
       </c>
@@ -11367,7 +10748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>4031</v>
       </c>
@@ -11474,7 +10855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>4032</v>
       </c>
@@ -11584,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>4033</v>
       </c>
@@ -11694,7 +11075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>4034</v>
       </c>
@@ -11804,7 +11185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>4035</v>
       </c>
@@ -11911,7 +11292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>4036</v>
       </c>
@@ -12018,7 +11399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:1026" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>4037</v>
       </c>
@@ -12126,8 +11507,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update TD config
调整对空增伤塔和buff升级效果，调整怪物模型
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E828EAB8-E264-4DF3-8F00-22F26F63E7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E226E2D-9866-4F02-BE3C-30C55BF6A80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="156">
   <si>
     <t>int</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>attackCount</t>
-  </si>
-  <si>
-    <t>speed</t>
   </si>
   <si>
     <t>speedPercent</t>
@@ -516,6 +513,10 @@
   </si>
   <si>
     <t>BD23066F40380CC8169768ADD657662A</t>
+  </si>
+  <si>
+    <t>speed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -906,11 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML64"/>
+  <dimension ref="A1:AML66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1124,61 +1125,61 @@
         <v>21</v>
       </c>
       <c r="S2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="AK2" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="AL2" s="5"/>
       <c r="AM2" s="5"/>
@@ -1190,115 +1191,115 @@
     </row>
     <row r="3" spans="1:44" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="Y3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Z3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AA3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AC3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AC3" s="21" t="s">
+      <c r="AD3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AF3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AG3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AI3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AJ3" s="6" t="s">
+      <c r="AK3" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
@@ -1310,7 +1311,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.35">
@@ -1329,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8">
@@ -1433,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8">
@@ -1639,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="3">
         <v>2</v>
@@ -1835,7 +1836,7 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3">
         <v>-1</v>
@@ -1938,7 +1939,7 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3">
         <v>-1</v>
@@ -2040,7 +2041,7 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="3">
         <v>-1</v>
@@ -2142,7 +2143,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3">
         <v>-1</v>
@@ -2244,7 +2245,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3">
         <v>-1</v>
@@ -2346,7 +2347,7 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E15" s="3">
         <v>-1</v>
@@ -2448,7 +2449,7 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" s="3">
         <v>-1</v>
@@ -2550,7 +2551,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="3">
         <v>-1</v>
@@ -2652,7 +2653,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="3">
         <v>-1</v>
@@ -2754,7 +2755,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E19" s="11">
         <v>2</v>
@@ -2763,10 +2764,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="I19" s="11">
         <v>1</v>
@@ -3852,7 +3853,7 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" s="11">
         <v>2</v>
@@ -3861,10 +3862,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I20" s="11">
         <v>1</v>
@@ -4950,7 +4951,7 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="11">
         <v>2</v>
@@ -4959,10 +4960,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I21" s="11">
         <v>1</v>
@@ -6047,10 +6048,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E22" s="3">
         <v>20</v>
@@ -6059,7 +6060,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="3">
         <v>1</v>
@@ -6154,10 +6155,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E23" s="3">
         <v>20</v>
@@ -6166,7 +6167,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I23" s="3">
         <v>1</v>
@@ -6261,10 +6262,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E24" s="3">
         <v>20</v>
@@ -6273,7 +6274,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I24" s="3">
         <v>1</v>
@@ -6368,7 +6369,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="3">
         <v>-1</v>
@@ -6469,7 +6470,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="3">
         <v>-1</v>
@@ -6570,7 +6571,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="3">
         <v>-1</v>
@@ -6671,7 +6672,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3">
         <v>3</v>
@@ -6772,7 +6773,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3">
         <v>3</v>
@@ -6873,7 +6874,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="3">
         <v>3</v>
@@ -6974,7 +6975,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -7075,7 +7076,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E32" s="3">
         <v>-1</v>
@@ -7176,7 +7177,7 @@
         <v>4009</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E33" s="3">
         <v>-1</v>
@@ -7277,7 +7278,7 @@
         <v>4010</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E34" s="3">
         <v>-1</v>
@@ -7378,7 +7379,7 @@
         <v>4011</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E35" s="3">
         <v>-1</v>
@@ -7479,7 +7480,7 @@
         <v>5001</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" s="3">
         <v>-1</v>
@@ -7580,7 +7581,7 @@
         <v>5002</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="3">
         <v>-1</v>
@@ -7681,7 +7682,7 @@
         <v>5003</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="3">
         <v>-1</v>
@@ -7782,7 +7783,7 @@
         <v>4012</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E39" s="3">
         <v>-1</v>
@@ -7883,7 +7884,7 @@
         <v>4013</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="3">
         <v>-1</v>
@@ -7984,7 +7985,7 @@
         <v>4014</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E41" s="3">
         <v>-1</v>
@@ -8085,7 +8086,7 @@
         <v>4015</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E42" s="3">
         <v>-1</v>
@@ -8186,7 +8187,7 @@
         <v>4016</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E43" s="3">
         <v>-1</v>
@@ -8287,7 +8288,7 @@
         <v>4017</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E44" s="3">
         <v>-1</v>
@@ -8388,7 +8389,7 @@
         <v>4018</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E45" s="3">
         <v>-1</v>
@@ -8489,7 +8490,7 @@
         <v>4019</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E46" s="3">
         <v>0.5</v>
@@ -8591,7 +8592,7 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -8693,7 +8694,7 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E48" s="3">
         <v>1</v>
@@ -8795,7 +8796,7 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E49" s="3">
         <v>1</v>
@@ -8897,19 +8898,19 @@
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="15">
+        <v>1</v>
+      </c>
+      <c r="F50" s="16">
+        <v>1</v>
+      </c>
+      <c r="G50" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E50" s="15">
-        <v>3</v>
-      </c>
-      <c r="F50" s="16">
-        <v>1</v>
-      </c>
-      <c r="G50" s="17" t="s">
+      <c r="H50" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="I50" s="15">
         <v>1</v>
@@ -9997,19 +9998,19 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
+      <c r="G51" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="3">
-        <v>3</v>
-      </c>
-      <c r="F51" s="9">
-        <v>1</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="H51" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I51" s="3">
         <v>1</v>
@@ -10108,19 +10109,19 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="9">
+        <v>1</v>
+      </c>
+      <c r="G52" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="E52" s="3">
-        <v>3</v>
-      </c>
-      <c r="F52" s="9">
-        <v>1</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="H52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I52" s="3">
         <v>1</v>
@@ -10219,19 +10220,19 @@
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1</v>
+      </c>
+      <c r="G53" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E53" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="H53" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I53" s="3">
         <v>1</v>
@@ -10327,19 +10328,19 @@
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="9">
+        <v>1</v>
+      </c>
+      <c r="G54" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="E54" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F54" s="9">
-        <v>1</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="H54" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I54" s="3">
         <v>1</v>
@@ -10435,19 +10436,19 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="9">
+        <v>1</v>
+      </c>
+      <c r="G55" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E55" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F55" s="9">
-        <v>1</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>137</v>
-      </c>
       <c r="H55" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I55" s="3">
         <v>1</v>
@@ -10542,19 +10543,19 @@
         <v>4029</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="E56" s="3">
-        <v>6</v>
-      </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>139</v>
-      </c>
       <c r="H56" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I56" s="3">
         <v>1</v>
@@ -10649,19 +10650,19 @@
         <v>4030</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="E57" s="3">
-        <v>6</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>141</v>
-      </c>
       <c r="H57" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I57" s="3">
         <v>1</v>
@@ -10756,19 +10757,19 @@
         <v>4031</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E58" s="3">
-        <v>6</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>143</v>
-      </c>
       <c r="H58" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I58" s="3">
         <v>1</v>
@@ -10863,19 +10864,19 @@
         <v>4032</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E59" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F59" s="3">
-        <v>1</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>145</v>
-      </c>
       <c r="H59" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I59" s="3">
         <v>1</v>
@@ -10973,19 +10974,19 @@
         <v>4033</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
+        <v>1</v>
+      </c>
+      <c r="G60" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>147</v>
-      </c>
       <c r="H60" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I60" s="3">
         <v>1</v>
@@ -11083,19 +11084,19 @@
         <v>4034</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
+      <c r="G61" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="E61" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F61" s="3">
-        <v>1</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="H61" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I61" s="3">
         <v>1</v>
@@ -11193,19 +11194,19 @@
         <v>4035</v>
       </c>
       <c r="D62" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E62" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="H62" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I62" s="3">
         <v>1</v>
@@ -11300,19 +11301,19 @@
         <v>4036</v>
       </c>
       <c r="D63" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="E63" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F63" s="3">
-        <v>1</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="H63" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I63" s="3">
         <v>1</v>
@@ -11407,19 +11408,19 @@
         <v>4037</v>
       </c>
       <c r="D64" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="G64" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E64" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F64" s="3">
-        <v>1</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>155</v>
-      </c>
       <c r="H64" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I64" s="3">
         <v>1</v>
@@ -11503,6 +11504,208 @@
         <v>0</v>
       </c>
       <c r="AK64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>4038</v>
+      </c>
+      <c r="B65" s="4">
+        <v>4038</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="I65" s="3">
+        <v>1</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+      <c r="M65" s="3">
+        <v>0</v>
+      </c>
+      <c r="N65" s="3">
+        <v>0</v>
+      </c>
+      <c r="O65" s="3">
+        <v>0</v>
+      </c>
+      <c r="P65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="3">
+        <v>0</v>
+      </c>
+      <c r="R65" s="3">
+        <v>0</v>
+      </c>
+      <c r="S65" s="3">
+        <v>0</v>
+      </c>
+      <c r="T65" s="3">
+        <v>0</v>
+      </c>
+      <c r="U65" s="3">
+        <v>0</v>
+      </c>
+      <c r="V65" s="3">
+        <v>0</v>
+      </c>
+      <c r="W65" s="3">
+        <v>0</v>
+      </c>
+      <c r="X65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A66" s="4">
+        <v>4039</v>
+      </c>
+      <c r="B66" s="4">
+        <v>4039</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E66" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3">
+        <v>1</v>
+      </c>
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3">
+        <v>0</v>
+      </c>
+      <c r="M66" s="3">
+        <v>0</v>
+      </c>
+      <c r="N66" s="3">
+        <v>0</v>
+      </c>
+      <c r="O66" s="3">
+        <v>0</v>
+      </c>
+      <c r="P66" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="3">
+        <v>0</v>
+      </c>
+      <c r="R66" s="3">
+        <v>0</v>
+      </c>
+      <c r="S66" s="3">
+        <v>0</v>
+      </c>
+      <c r="T66" s="3">
+        <v>0</v>
+      </c>
+      <c r="U66" s="3">
+        <v>0</v>
+      </c>
+      <c r="V66" s="3">
+        <v>0</v>
+      </c>
+      <c r="W66" s="3">
+        <v>0</v>
+      </c>
+      <c r="X66" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA66" s="3">
+        <v>30</v>
+      </c>
+      <c r="AB66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ66" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK66" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: change slow buff
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E226E2D-9866-4F02-BE3C-30C55BF6A80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -99,6 +95,9 @@
     <t>attackCount</t>
   </si>
   <si>
+    <t>speed</t>
+  </si>
+  <si>
     <t>speedPercent</t>
   </si>
   <si>
@@ -513,17 +512,19 @@
   </si>
   <si>
     <t>BD23066F40380CC8169768ADD657662A</t>
-  </si>
-  <si>
-    <t>speed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -533,13 +534,11 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -547,27 +546,18 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -575,11 +565,161 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,7 +734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
@@ -606,7 +746,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,8 +756,194 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -651,9 +977,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -701,9 +1269,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -713,10 +1281,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -790,9 +1405,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -850,7 +1462,7 @@
         <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -901,20 +1513,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AML66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N58" sqref="N58"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.75" style="3" customWidth="1"/>
@@ -930,7 +1543,7 @@
     <col min="16" max="16" width="10.5" style="3" customWidth="1"/>
     <col min="17" max="17" width="16.5" style="3" customWidth="1"/>
     <col min="18" max="18" width="11.25" style="3" customWidth="1"/>
-    <col min="19" max="19" width="6.25" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.125" style="3" customWidth="1"/>
     <col min="20" max="20" width="12.375" style="3" customWidth="1"/>
     <col min="21" max="21" width="7.875" style="3" customWidth="1"/>
     <col min="22" max="22" width="11.25" style="3" customWidth="1"/>
@@ -949,7 +1562,7 @@
     <col min="36" max="1026" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" ht="26.25" customHeight="1" spans="1:44">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1682,7 @@
       <c r="AQ1" s="5"/>
       <c r="AR1" s="5"/>
     </row>
-    <row r="2" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" ht="24.75" customHeight="1" spans="1:44">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1125,61 +1738,61 @@
         <v>21</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AL2" s="5"/>
       <c r="AM2" s="5"/>
@@ -1189,117 +1802,117 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:44" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" ht="105" customHeight="1" spans="1:44">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC3" s="21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AH3" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
@@ -1309,12 +1922,12 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" ht="16.5" spans="3:3">
       <c r="C4" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37">
       <c r="A5" s="4">
         <v>1001</v>
       </c>
@@ -1330,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8">
@@ -1418,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37">
       <c r="A6" s="4">
         <v>1002</v>
       </c>
@@ -1434,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8">
@@ -1522,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37">
       <c r="A7" s="4">
         <v>1003</v>
       </c>
@@ -1624,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37">
       <c r="A8" s="4">
         <v>1004</v>
       </c>
@@ -1640,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I8" s="3">
         <v>2</v>
@@ -1727,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37">
       <c r="A9" s="4">
         <v>1005</v>
       </c>
@@ -1827,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37">
       <c r="A10" s="4">
         <v>1006</v>
       </c>
@@ -1836,7 +2449,7 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E10" s="3">
         <v>-1</v>
@@ -1930,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37">
       <c r="A11" s="4">
         <v>1007</v>
       </c>
@@ -1939,7 +2552,7 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E11" s="3">
         <v>-1</v>
@@ -2032,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37">
       <c r="A12" s="4">
         <v>1008</v>
       </c>
@@ -2041,7 +2654,7 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3">
         <v>-1</v>
@@ -2134,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37">
       <c r="A13" s="4">
         <v>1009</v>
       </c>
@@ -2143,7 +2756,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E13" s="3">
         <v>-1</v>
@@ -2236,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37">
       <c r="A14" s="4">
         <v>1010</v>
       </c>
@@ -2245,7 +2858,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E14" s="3">
         <v>-1</v>
@@ -2338,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37">
       <c r="A15" s="4">
         <v>1011</v>
       </c>
@@ -2347,7 +2960,7 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E15" s="3">
         <v>-1</v>
@@ -2383,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="S15" s="20">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="T15" s="3">
         <v>0</v>
@@ -2440,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37">
       <c r="A16" s="4">
         <v>1012</v>
       </c>
@@ -2449,7 +3062,7 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E16" s="3">
         <v>-1</v>
@@ -2542,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37">
       <c r="A17" s="4">
         <v>1013</v>
       </c>
@@ -2551,7 +3164,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3">
         <v>-1</v>
@@ -2644,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37">
       <c r="A18" s="4">
         <v>1014</v>
       </c>
@@ -2653,7 +3266,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" s="3">
         <v>-1</v>
@@ -2746,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" s="1" customFormat="1" spans="1:1026">
       <c r="A19" s="10">
         <v>2001</v>
       </c>
@@ -2755,7 +3368,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E19" s="11">
         <v>2</v>
@@ -2764,10 +3377,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I19" s="11">
         <v>1</v>
@@ -3844,7 +4457,7 @@
       <c r="AMK19" s="11"/>
       <c r="AML19" s="11"/>
     </row>
-    <row r="20" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" s="1" customFormat="1" spans="1:1026">
       <c r="A20" s="10">
         <v>2002</v>
       </c>
@@ -3853,7 +4466,7 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E20" s="11">
         <v>2</v>
@@ -3862,10 +4475,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I20" s="11">
         <v>1</v>
@@ -4942,7 +5555,7 @@
       <c r="AMK20" s="11"/>
       <c r="AML20" s="11"/>
     </row>
-    <row r="21" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" s="1" customFormat="1" spans="1:1026">
       <c r="A21" s="10">
         <v>2003</v>
       </c>
@@ -4951,7 +5564,7 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21" s="11">
         <v>2</v>
@@ -4960,10 +5573,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I21" s="11">
         <v>1</v>
@@ -6040,7 +6653,7 @@
       <c r="AMK21" s="11"/>
       <c r="AML21" s="11"/>
     </row>
-    <row r="22" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="22" ht="15.5" spans="1:37">
       <c r="A22" s="3">
         <v>3001</v>
       </c>
@@ -6048,10 +6661,10 @@
         <v>3001</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E22" s="3">
         <v>20</v>
@@ -6060,7 +6673,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I22" s="3">
         <v>1</v>
@@ -6147,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="23" ht="15.5" spans="1:37">
       <c r="A23" s="3">
         <v>3002</v>
       </c>
@@ -6155,10 +6768,10 @@
         <v>3002</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E23" s="3">
         <v>20</v>
@@ -6167,7 +6780,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I23" s="3">
         <v>1</v>
@@ -6254,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="24" ht="15.5" spans="1:37">
       <c r="A24" s="3">
         <v>3003</v>
       </c>
@@ -6262,10 +6875,10 @@
         <v>3003</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E24" s="3">
         <v>20</v>
@@ -6274,7 +6887,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I24" s="3">
         <v>1</v>
@@ -6361,7 +6974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:37">
       <c r="A25" s="3">
         <v>4001</v>
       </c>
@@ -6369,7 +6982,7 @@
         <v>4001</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E25" s="3">
         <v>-1</v>
@@ -6462,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37">
       <c r="A26" s="3">
         <v>4002</v>
       </c>
@@ -6470,7 +7083,7 @@
         <v>4002</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3">
         <v>-1</v>
@@ -6563,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:37">
       <c r="A27" s="3">
         <v>4003</v>
       </c>
@@ -6571,7 +7184,7 @@
         <v>4003</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3">
         <v>-1</v>
@@ -6664,7 +7277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:37">
       <c r="A28" s="3">
         <v>4004</v>
       </c>
@@ -6672,7 +7285,7 @@
         <v>4004</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E28" s="3">
         <v>3</v>
@@ -6765,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:37">
       <c r="A29" s="3">
         <v>4005</v>
       </c>
@@ -6773,7 +7386,7 @@
         <v>4005</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="3">
         <v>3</v>
@@ -6866,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:37">
       <c r="A30" s="3">
         <v>4006</v>
       </c>
@@ -6874,7 +7487,7 @@
         <v>4006</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E30" s="3">
         <v>3</v>
@@ -6910,7 +7523,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="3">
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="T30" s="3">
         <v>0</v>
@@ -6967,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:37">
       <c r="A31" s="3">
         <v>4007</v>
       </c>
@@ -6975,7 +7588,7 @@
         <v>4007</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -7011,7 +7624,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="3">
-        <v>-999</v>
+        <v>999</v>
       </c>
       <c r="T31" s="3">
         <v>0</v>
@@ -7068,7 +7681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:37">
       <c r="A32" s="3">
         <v>4008</v>
       </c>
@@ -7076,7 +7689,7 @@
         <v>4008</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E32" s="3">
         <v>-1</v>
@@ -7169,7 +7782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:37">
       <c r="A33" s="3">
         <v>4009</v>
       </c>
@@ -7177,7 +7790,7 @@
         <v>4009</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E33" s="3">
         <v>-1</v>
@@ -7270,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:37">
       <c r="A34" s="3">
         <v>4010</v>
       </c>
@@ -7278,7 +7891,7 @@
         <v>4010</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34" s="3">
         <v>-1</v>
@@ -7371,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:37">
       <c r="A35" s="3">
         <v>4011</v>
       </c>
@@ -7379,7 +7992,7 @@
         <v>4011</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E35" s="3">
         <v>-1</v>
@@ -7472,7 +8085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:37">
       <c r="A36" s="3">
         <v>5001</v>
       </c>
@@ -7480,7 +8093,7 @@
         <v>5001</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E36" s="3">
         <v>-1</v>
@@ -7573,7 +8186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:37">
       <c r="A37" s="3">
         <v>5002</v>
       </c>
@@ -7581,7 +8194,7 @@
         <v>5002</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E37" s="3">
         <v>-1</v>
@@ -7674,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:37">
       <c r="A38" s="3">
         <v>5003</v>
       </c>
@@ -7682,7 +8295,7 @@
         <v>5003</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E38" s="3">
         <v>-1</v>
@@ -7775,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:37">
       <c r="A39" s="3">
         <v>4012</v>
       </c>
@@ -7783,7 +8396,7 @@
         <v>4012</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E39" s="3">
         <v>-1</v>
@@ -7876,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:37">
       <c r="A40" s="3">
         <v>4013</v>
       </c>
@@ -7884,7 +8497,7 @@
         <v>4013</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E40" s="3">
         <v>-1</v>
@@ -7977,7 +8590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:37">
       <c r="A41" s="3">
         <v>4014</v>
       </c>
@@ -7985,7 +8598,7 @@
         <v>4014</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E41" s="3">
         <v>-1</v>
@@ -8078,7 +8691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:37">
       <c r="A42" s="3">
         <v>4015</v>
       </c>
@@ -8086,7 +8699,7 @@
         <v>4015</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E42" s="3">
         <v>-1</v>
@@ -8179,7 +8792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:37">
       <c r="A43" s="3">
         <v>4016</v>
       </c>
@@ -8187,7 +8800,7 @@
         <v>4016</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E43" s="3">
         <v>-1</v>
@@ -8280,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:37">
       <c r="A44" s="3">
         <v>4017</v>
       </c>
@@ -8288,7 +8901,7 @@
         <v>4017</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E44" s="3">
         <v>-1</v>
@@ -8381,7 +8994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:37">
       <c r="A45" s="3">
         <v>4018</v>
       </c>
@@ -8389,7 +9002,7 @@
         <v>4018</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E45" s="3">
         <v>-1</v>
@@ -8482,7 +9095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37">
       <c r="A46" s="3">
         <v>4019</v>
       </c>
@@ -8490,7 +9103,7 @@
         <v>4019</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E46" s="3">
         <v>0.5</v>
@@ -8526,7 +9139,7 @@
         <v>0</v>
       </c>
       <c r="S46" s="3">
-        <v>-999</v>
+        <v>999</v>
       </c>
       <c r="T46" s="3">
         <v>0</v>
@@ -8583,7 +9196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37">
       <c r="A47" s="4">
         <v>4020</v>
       </c>
@@ -8592,7 +9205,7 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -8628,7 +9241,7 @@
         <v>0</v>
       </c>
       <c r="S47" s="20">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="T47" s="3">
         <v>0</v>
@@ -8685,7 +9298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:37">
       <c r="A48" s="4">
         <v>4021</v>
       </c>
@@ -8694,7 +9307,7 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E48" s="3">
         <v>1</v>
@@ -8730,7 +9343,7 @@
         <v>0</v>
       </c>
       <c r="S48" s="20">
-        <v>-15</v>
+        <v>15</v>
       </c>
       <c r="T48" s="3">
         <v>0</v>
@@ -8787,7 +9400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:37">
       <c r="A49" s="4">
         <v>4022</v>
       </c>
@@ -8796,7 +9409,7 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E49" s="3">
         <v>1</v>
@@ -8832,7 +9445,7 @@
         <v>0</v>
       </c>
       <c r="S49" s="20">
-        <v>-20</v>
+        <v>20</v>
       </c>
       <c r="T49" s="3">
         <v>0</v>
@@ -8889,7 +9502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" s="2" customFormat="1" spans="1:1026">
       <c r="A50" s="14">
         <v>4023</v>
       </c>
@@ -8898,7 +9511,7 @@
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E50" s="15">
         <v>1</v>
@@ -8907,10 +9520,10 @@
         <v>1</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I50" s="15">
         <v>1</v>
@@ -9989,7 +10602,7 @@
       <c r="AMK50" s="15"/>
       <c r="AML50" s="15"/>
     </row>
-    <row r="51" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:37">
       <c r="A51" s="4">
         <v>4024</v>
       </c>
@@ -9998,19 +10611,19 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="E51" s="3">
-        <v>1</v>
-      </c>
-      <c r="F51" s="9">
-        <v>1</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="I51" s="3">
         <v>1</v>
@@ -10100,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:37">
       <c r="A52" s="4">
         <v>4025</v>
       </c>
@@ -10109,7 +10722,7 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
@@ -10118,10 +10731,10 @@
         <v>1</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I52" s="3">
         <v>1</v>
@@ -10211,7 +10824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:37">
       <c r="A53" s="4">
         <v>4026</v>
       </c>
@@ -10220,7 +10833,7 @@
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -10229,10 +10842,10 @@
         <v>1</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I53" s="3">
         <v>1</v>
@@ -10319,7 +10932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:37">
       <c r="A54" s="4">
         <v>4027</v>
       </c>
@@ -10328,7 +10941,7 @@
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E54" s="3">
         <v>1</v>
@@ -10337,10 +10950,10 @@
         <v>1</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I54" s="3">
         <v>1</v>
@@ -10427,7 +11040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:37">
       <c r="A55" s="4">
         <v>4028</v>
       </c>
@@ -10436,7 +11049,7 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E55" s="3">
         <v>1</v>
@@ -10445,10 +11058,10 @@
         <v>1</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I55" s="3">
         <v>1</v>
@@ -10535,7 +11148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:37">
       <c r="A56" s="4">
         <v>4029</v>
       </c>
@@ -10543,7 +11156,7 @@
         <v>4029</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E56" s="3">
         <v>1</v>
@@ -10552,10 +11165,10 @@
         <v>1</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I56" s="3">
         <v>1</v>
@@ -10642,7 +11255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:37">
       <c r="A57" s="4">
         <v>4030</v>
       </c>
@@ -10650,7 +11263,7 @@
         <v>4030</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E57" s="3">
         <v>1</v>
@@ -10659,10 +11272,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I57" s="3">
         <v>1</v>
@@ -10749,7 +11362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:37">
       <c r="A58" s="4">
         <v>4031</v>
       </c>
@@ -10757,7 +11370,7 @@
         <v>4031</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E58" s="3">
         <v>1</v>
@@ -10766,10 +11379,10 @@
         <v>1</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I58" s="3">
         <v>1</v>
@@ -10856,7 +11469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:37">
       <c r="A59" s="4">
         <v>4032</v>
       </c>
@@ -10864,7 +11477,7 @@
         <v>4032</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E59" s="3">
         <v>1</v>
@@ -10873,10 +11486,10 @@
         <v>1</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I59" s="3">
         <v>1</v>
@@ -10966,7 +11579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:37">
       <c r="A60" s="4">
         <v>4033</v>
       </c>
@@ -10974,7 +11587,7 @@
         <v>4033</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E60" s="3">
         <v>1</v>
@@ -10983,10 +11596,10 @@
         <v>1</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I60" s="3">
         <v>1</v>
@@ -11076,7 +11689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:37">
       <c r="A61" s="4">
         <v>4034</v>
       </c>
@@ -11084,7 +11697,7 @@
         <v>4034</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E61" s="3">
         <v>1</v>
@@ -11093,10 +11706,10 @@
         <v>1</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I61" s="3">
         <v>1</v>
@@ -11186,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:37">
       <c r="A62" s="4">
         <v>4035</v>
       </c>
@@ -11194,7 +11807,7 @@
         <v>4035</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E62" s="3">
         <v>1</v>
@@ -11203,10 +11816,10 @@
         <v>1</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I62" s="3">
         <v>1</v>
@@ -11293,7 +11906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:37">
       <c r="A63" s="4">
         <v>4036</v>
       </c>
@@ -11301,7 +11914,7 @@
         <v>4036</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E63" s="3">
         <v>1</v>
@@ -11310,10 +11923,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I63" s="3">
         <v>1</v>
@@ -11400,7 +12013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:1026" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:37">
       <c r="A64" s="4">
         <v>4037</v>
       </c>
@@ -11408,7 +12021,7 @@
         <v>4037</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E64" s="3">
         <v>1</v>
@@ -11417,10 +12030,10 @@
         <v>1</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I64" s="3">
         <v>1</v>
@@ -11507,7 +12120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:37">
       <c r="A65" s="4">
         <v>4038</v>
       </c>
@@ -11515,7 +12128,7 @@
         <v>4038</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E65" s="3">
         <v>-1</v>
@@ -11608,7 +12221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:37">
       <c r="A66" s="4">
         <v>4039</v>
       </c>
@@ -11616,7 +12229,7 @@
         <v>4039</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E66" s="3">
         <v>-1</v>
@@ -11710,8 +12323,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update Asset Config
关闭新手村内音效节点 调整怪物行走动作
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D11594-58FA-4B49-8675-CC8B3D6760B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E05F06-AF95-498F-949A-D890A4B01035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat: update task buff tower
更新部分塔 更新buff 更新任务奖励 更新世界3波次奖励
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Buff_buff表.xlsx
+++ b/nevergiveup/Excel/Buff_buff表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E05F06-AF95-498F-949A-D890A4B01035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CE0B8B-4A02-40ED-B7B7-0C556FC3A426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="159">
   <si>
     <t>int</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t>BD23066F40380CC8169768ADD657662A</t>
+  </si>
+  <si>
+    <t>50物穿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60物穿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>70物穿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -900,11 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML66"/>
+  <dimension ref="A1:AML74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -10234,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="3">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="M53" s="3">
         <v>0</v>
@@ -10342,7 +10354,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M54" s="3">
         <v>0</v>
@@ -10450,7 +10462,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="M55" s="3">
         <v>0</v>
@@ -11699,6 +11711,814 @@
         <v>0</v>
       </c>
       <c r="AK66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A67" s="4">
+        <v>4040</v>
+      </c>
+      <c r="B67" s="4">
+        <v>4040</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E67" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="I67" s="3">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0</v>
+      </c>
+      <c r="M67" s="3">
+        <v>0</v>
+      </c>
+      <c r="N67" s="3">
+        <v>0</v>
+      </c>
+      <c r="O67" s="3">
+        <v>0</v>
+      </c>
+      <c r="P67" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="3">
+        <v>0</v>
+      </c>
+      <c r="R67" s="3">
+        <v>0</v>
+      </c>
+      <c r="S67" s="3">
+        <v>0</v>
+      </c>
+      <c r="T67" s="3">
+        <v>0</v>
+      </c>
+      <c r="U67" s="3">
+        <v>0</v>
+      </c>
+      <c r="V67" s="3">
+        <v>0</v>
+      </c>
+      <c r="W67" s="20">
+        <v>50</v>
+      </c>
+      <c r="X67" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A68" s="4">
+        <v>4041</v>
+      </c>
+      <c r="B68" s="4">
+        <v>4041</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E68" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3">
+        <v>1</v>
+      </c>
+      <c r="J68" s="3">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+      <c r="M68" s="3">
+        <v>0</v>
+      </c>
+      <c r="N68" s="3">
+        <v>0</v>
+      </c>
+      <c r="O68" s="3">
+        <v>0</v>
+      </c>
+      <c r="P68" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="3">
+        <v>0</v>
+      </c>
+      <c r="R68" s="3">
+        <v>0</v>
+      </c>
+      <c r="S68" s="3">
+        <v>0</v>
+      </c>
+      <c r="T68" s="3">
+        <v>0</v>
+      </c>
+      <c r="U68" s="3">
+        <v>0</v>
+      </c>
+      <c r="V68" s="3">
+        <v>0</v>
+      </c>
+      <c r="W68" s="20">
+        <v>60</v>
+      </c>
+      <c r="X68" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ68" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A69" s="4">
+        <v>4042</v>
+      </c>
+      <c r="B69" s="4">
+        <v>4042</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E69" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3">
+        <v>1</v>
+      </c>
+      <c r="J69" s="3">
+        <v>0</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+      <c r="N69" s="3">
+        <v>0</v>
+      </c>
+      <c r="O69" s="3">
+        <v>0</v>
+      </c>
+      <c r="P69" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="3">
+        <v>0</v>
+      </c>
+      <c r="R69" s="3">
+        <v>0</v>
+      </c>
+      <c r="S69" s="3">
+        <v>0</v>
+      </c>
+      <c r="T69" s="3">
+        <v>0</v>
+      </c>
+      <c r="U69" s="3">
+        <v>0</v>
+      </c>
+      <c r="V69" s="3">
+        <v>0</v>
+      </c>
+      <c r="W69" s="20">
+        <v>70</v>
+      </c>
+      <c r="X69" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ69" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A70" s="4">
+        <v>4043</v>
+      </c>
+      <c r="B70" s="4">
+        <v>4043</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E70" s="3">
+        <v>3</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1</v>
+      </c>
+      <c r="I70" s="3">
+        <v>2</v>
+      </c>
+      <c r="J70" s="3">
+        <v>0</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+      <c r="N70" s="3">
+        <v>0</v>
+      </c>
+      <c r="O70" s="3">
+        <v>0</v>
+      </c>
+      <c r="P70" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="3">
+        <v>0</v>
+      </c>
+      <c r="R70" s="3">
+        <v>0</v>
+      </c>
+      <c r="S70" s="3">
+        <v>0</v>
+      </c>
+      <c r="T70" s="3">
+        <v>0</v>
+      </c>
+      <c r="U70" s="3">
+        <v>0</v>
+      </c>
+      <c r="V70" s="3">
+        <v>0</v>
+      </c>
+      <c r="W70" s="3">
+        <v>0</v>
+      </c>
+      <c r="X70" s="3">
+        <v>70</v>
+      </c>
+      <c r="Y70" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ70" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A71" s="4">
+        <v>4044</v>
+      </c>
+      <c r="B71" s="4">
+        <v>4044</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E71" s="3">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="I71" s="3">
+        <v>2</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0</v>
+      </c>
+      <c r="L71" s="3">
+        <v>0</v>
+      </c>
+      <c r="M71" s="3">
+        <v>0</v>
+      </c>
+      <c r="N71" s="3">
+        <v>0</v>
+      </c>
+      <c r="O71" s="3">
+        <v>0</v>
+      </c>
+      <c r="P71" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="3">
+        <v>0</v>
+      </c>
+      <c r="R71" s="3">
+        <v>0</v>
+      </c>
+      <c r="S71" s="3">
+        <v>0</v>
+      </c>
+      <c r="T71" s="3">
+        <v>0</v>
+      </c>
+      <c r="U71" s="3">
+        <v>0</v>
+      </c>
+      <c r="V71" s="3">
+        <v>0</v>
+      </c>
+      <c r="W71" s="3">
+        <v>0</v>
+      </c>
+      <c r="X71" s="3">
+        <v>85</v>
+      </c>
+      <c r="Y71" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A72" s="4">
+        <v>4045</v>
+      </c>
+      <c r="B72" s="4">
+        <v>4045</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E72" s="3">
+        <v>3</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="I72" s="3">
+        <v>2</v>
+      </c>
+      <c r="J72" s="3">
+        <v>0</v>
+      </c>
+      <c r="L72" s="3">
+        <v>0</v>
+      </c>
+      <c r="M72" s="3">
+        <v>0</v>
+      </c>
+      <c r="N72" s="3">
+        <v>0</v>
+      </c>
+      <c r="O72" s="3">
+        <v>0</v>
+      </c>
+      <c r="P72" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>0</v>
+      </c>
+      <c r="R72" s="3">
+        <v>0</v>
+      </c>
+      <c r="S72" s="3">
+        <v>0</v>
+      </c>
+      <c r="T72" s="3">
+        <v>0</v>
+      </c>
+      <c r="U72" s="3">
+        <v>0</v>
+      </c>
+      <c r="V72" s="3">
+        <v>0</v>
+      </c>
+      <c r="W72" s="3">
+        <v>0</v>
+      </c>
+      <c r="X72" s="3">
+        <v>30</v>
+      </c>
+      <c r="Y72" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A73" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B73" s="4">
+        <v>4046</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E73" s="3">
+        <v>3</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="I73" s="3">
+        <v>2</v>
+      </c>
+      <c r="J73" s="3">
+        <v>0</v>
+      </c>
+      <c r="L73" s="3">
+        <v>0</v>
+      </c>
+      <c r="M73" s="3">
+        <v>0</v>
+      </c>
+      <c r="N73" s="3">
+        <v>0</v>
+      </c>
+      <c r="O73" s="3">
+        <v>0</v>
+      </c>
+      <c r="P73" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="3">
+        <v>0</v>
+      </c>
+      <c r="R73" s="3">
+        <v>0</v>
+      </c>
+      <c r="S73" s="3">
+        <v>0</v>
+      </c>
+      <c r="T73" s="3">
+        <v>0</v>
+      </c>
+      <c r="U73" s="3">
+        <v>0</v>
+      </c>
+      <c r="V73" s="3">
+        <v>0</v>
+      </c>
+      <c r="W73" s="3">
+        <v>0</v>
+      </c>
+      <c r="X73" s="3">
+        <v>35</v>
+      </c>
+      <c r="Y73" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A74" s="4">
+        <v>4047</v>
+      </c>
+      <c r="B74" s="4">
+        <v>4047</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E74" s="3">
+        <v>3</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="I74" s="3">
+        <v>2</v>
+      </c>
+      <c r="J74" s="3">
+        <v>0</v>
+      </c>
+      <c r="L74" s="3">
+        <v>0</v>
+      </c>
+      <c r="M74" s="3">
+        <v>0</v>
+      </c>
+      <c r="N74" s="3">
+        <v>0</v>
+      </c>
+      <c r="O74" s="3">
+        <v>0</v>
+      </c>
+      <c r="P74" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="3">
+        <v>0</v>
+      </c>
+      <c r="R74" s="3">
+        <v>0</v>
+      </c>
+      <c r="S74" s="3">
+        <v>0</v>
+      </c>
+      <c r="T74" s="3">
+        <v>0</v>
+      </c>
+      <c r="U74" s="3">
+        <v>0</v>
+      </c>
+      <c r="V74" s="3">
+        <v>0</v>
+      </c>
+      <c r="W74" s="3">
+        <v>0</v>
+      </c>
+      <c r="X74" s="3">
+        <v>40</v>
+      </c>
+      <c r="Y74" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ74" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK74" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>